<commit_message>
finished arbeitsjournal and zeitplan for today
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FD7289-8497-4432-9B09-10828C0DA5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AB375E-BDA4-4407-915A-35521C84CEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -935,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1219,6 +1219,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1533,7 +1534,7 @@
   <dimension ref="A1:AS91"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E26" sqref="E26:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,7 +2958,9 @@
       <c r="D26" s="62">
         <v>1</v>
       </c>
-      <c r="E26" s="63"/>
+      <c r="E26" s="63">
+        <v>1</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -3011,7 +3014,7 @@
       <c r="I27" s="18"/>
       <c r="J27" s="16"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
+      <c r="L27" s="131"/>
       <c r="M27" s="18"/>
       <c r="N27" s="16"/>
       <c r="O27" s="17"/>
@@ -5664,7 +5667,7 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>

</xml_diff>

<commit_message>
updated zeitplan, finished arbeitspaket 14
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AB375E-BDA4-4407-915A-35521C84CEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCD0A04-73B4-4710-B37E-F2C9972BCE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -935,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1007,219 +1007,221 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1534,7 +1536,7 @@
   <dimension ref="A1:AS91"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:E27"/>
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,151 +1553,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="80" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="80" t="s">
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="80" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="80" t="s">
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="80" t="s">
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="80" t="s">
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="80" t="s">
+      <c r="AA1" s="88"/>
+      <c r="AB1" s="88"/>
+      <c r="AC1" s="89"/>
+      <c r="AD1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="80" t="s">
+      <c r="AE1" s="88"/>
+      <c r="AF1" s="88"/>
+      <c r="AG1" s="89"/>
+      <c r="AH1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="81"/>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="80" t="s">
+      <c r="AI1" s="88"/>
+      <c r="AJ1" s="88"/>
+      <c r="AK1" s="89"/>
+      <c r="AL1" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="81"/>
-      <c r="AN1" s="81"/>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="95" t="s">
+      <c r="AM1" s="88"/>
+      <c r="AN1" s="88"/>
+      <c r="AO1" s="89"/>
+      <c r="AP1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="96"/>
-      <c r="AS1" s="97"/>
+      <c r="AQ1" s="103"/>
+      <c r="AR1" s="103"/>
+      <c r="AS1" s="104"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A2" s="90"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="92">
+      <c r="A2" s="126"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="99">
         <v>45351</v>
       </c>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="92">
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="99">
         <v>45355</v>
       </c>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="92">
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="99">
         <v>45356</v>
       </c>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="92">
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="99">
         <v>45357</v>
       </c>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="94"/>
-      <c r="V2" s="92">
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="101"/>
+      <c r="V2" s="99">
         <v>45358</v>
       </c>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="94"/>
-      <c r="Z2" s="92">
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="101"/>
+      <c r="Z2" s="99">
         <v>45362</v>
       </c>
-      <c r="AA2" s="93"/>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="94"/>
-      <c r="AD2" s="92">
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="100"/>
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="99">
         <v>45363</v>
       </c>
-      <c r="AE2" s="93"/>
-      <c r="AF2" s="93"/>
-      <c r="AG2" s="94"/>
-      <c r="AH2" s="92">
+      <c r="AE2" s="100"/>
+      <c r="AF2" s="100"/>
+      <c r="AG2" s="101"/>
+      <c r="AH2" s="99">
         <v>45364</v>
       </c>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="94"/>
-      <c r="AL2" s="92">
+      <c r="AI2" s="100"/>
+      <c r="AJ2" s="100"/>
+      <c r="AK2" s="101"/>
+      <c r="AL2" s="99">
         <v>45365</v>
       </c>
-      <c r="AM2" s="93"/>
-      <c r="AN2" s="93"/>
-      <c r="AO2" s="94"/>
-      <c r="AP2" s="92">
+      <c r="AM2" s="100"/>
+      <c r="AN2" s="100"/>
+      <c r="AO2" s="101"/>
+      <c r="AP2" s="99">
         <v>45369</v>
       </c>
-      <c r="AQ2" s="93"/>
-      <c r="AR2" s="93"/>
-      <c r="AS2" s="94"/>
+      <c r="AQ2" s="100"/>
+      <c r="AR2" s="100"/>
+      <c r="AS2" s="101"/>
     </row>
     <row r="3" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="100"/>
+      <c r="A3" s="127"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1824,17 +1826,17 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="83"/>
-      <c r="B4" s="61">
+      <c r="A4" s="120"/>
+      <c r="B4" s="78">
         <v>0</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="74">
         <v>25</v>
       </c>
-      <c r="E4" s="63"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -1873,27 +1875,27 @@
       <c r="AO4" s="26"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="25"/>
-      <c r="AR4" s="105" t="s">
+      <c r="AR4" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="AS4" s="106"/>
+      <c r="AS4" s="114"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="53"/>
       <c r="G5" s="54"/>
       <c r="H5" s="54"/>
       <c r="I5" s="58"/>
       <c r="J5" s="30"/>
       <c r="K5" s="31"/>
-      <c r="L5" s="130"/>
-      <c r="M5" s="32"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="63"/>
       <c r="N5" s="30"/>
-      <c r="O5" s="31"/>
+      <c r="O5" s="60"/>
       <c r="P5" s="31"/>
       <c r="Q5" s="32"/>
       <c r="R5" s="33"/>
@@ -1922,21 +1924,21 @@
       <c r="AO5" s="29"/>
       <c r="AP5" s="33"/>
       <c r="AQ5" s="28"/>
-      <c r="AR5" s="107"/>
-      <c r="AS5" s="108"/>
+      <c r="AR5" s="115"/>
+      <c r="AS5" s="116"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="61">
+      <c r="A6" s="77"/>
+      <c r="B6" s="78">
         <v>1</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="74">
         <v>1</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="65">
         <v>1</v>
       </c>
       <c r="F6" s="38"/>
@@ -1977,15 +1979,15 @@
       <c r="AO6" s="10"/>
       <c r="AP6" s="8"/>
       <c r="AQ6" s="9"/>
-      <c r="AR6" s="107"/>
-      <c r="AS6" s="108"/>
+      <c r="AR6" s="115"/>
+      <c r="AS6" s="116"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="53"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -2024,21 +2026,21 @@
       <c r="AO7" s="10"/>
       <c r="AP7" s="8"/>
       <c r="AQ7" s="9"/>
-      <c r="AR7" s="107"/>
-      <c r="AS7" s="108"/>
+      <c r="AR7" s="115"/>
+      <c r="AS7" s="116"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="61">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78">
         <v>2</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="74">
         <v>2</v>
       </c>
-      <c r="E8" s="63"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="33"/>
       <c r="G8" s="28"/>
       <c r="H8" s="9"/>
@@ -2077,15 +2079,15 @@
       <c r="AO8" s="10"/>
       <c r="AP8" s="33"/>
       <c r="AQ8" s="37"/>
-      <c r="AR8" s="107"/>
-      <c r="AS8" s="108"/>
+      <c r="AR8" s="115"/>
+      <c r="AS8" s="116"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="65"/>
       <c r="F9" s="33"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2124,21 +2126,21 @@
       <c r="AO9" s="10"/>
       <c r="AP9" s="8"/>
       <c r="AQ9" s="9"/>
-      <c r="AR9" s="107"/>
-      <c r="AS9" s="108"/>
+      <c r="AR9" s="115"/>
+      <c r="AS9" s="116"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="61">
+      <c r="A10" s="77"/>
+      <c r="B10" s="78">
         <v>3</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="74">
         <v>1</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="65">
         <v>0.5</v>
       </c>
       <c r="F10" s="8"/>
@@ -2179,15 +2181,15 @@
       <c r="AO10" s="55"/>
       <c r="AP10" s="8"/>
       <c r="AQ10" s="9"/>
-      <c r="AR10" s="107"/>
-      <c r="AS10" s="108"/>
+      <c r="AR10" s="115"/>
+      <c r="AS10" s="116"/>
     </row>
     <row r="11" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="114"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="119"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2226,23 +2228,23 @@
       <c r="AO11" s="14"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="13"/>
-      <c r="AR11" s="107"/>
-      <c r="AS11" s="108"/>
+      <c r="AR11" s="115"/>
+      <c r="AS11" s="116"/>
     </row>
     <row r="12" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="61">
+      <c r="B12" s="78">
         <v>4</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="116">
+      <c r="D12" s="73">
         <v>1</v>
       </c>
-      <c r="E12" s="117">
+      <c r="E12" s="75">
         <v>1</v>
       </c>
       <c r="F12" s="40"/>
@@ -2283,15 +2285,15 @@
       <c r="AO12" s="15"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="7"/>
-      <c r="AR12" s="107"/>
-      <c r="AS12" s="108"/>
+      <c r="AR12" s="115"/>
+      <c r="AS12" s="116"/>
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="33"/>
       <c r="G13" s="54"/>
       <c r="H13" s="28"/>
@@ -2330,21 +2332,21 @@
       <c r="AO13" s="10"/>
       <c r="AP13" s="8"/>
       <c r="AQ13" s="9"/>
-      <c r="AR13" s="107"/>
-      <c r="AS13" s="108"/>
+      <c r="AR13" s="115"/>
+      <c r="AS13" s="116"/>
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="61">
+      <c r="A14" s="77"/>
+      <c r="B14" s="78">
         <v>5</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="62">
+      <c r="D14" s="74">
         <v>1</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="65">
         <v>1</v>
       </c>
       <c r="F14" s="8"/>
@@ -2385,15 +2387,15 @@
       <c r="AO14" s="10"/>
       <c r="AP14" s="8"/>
       <c r="AQ14" s="9"/>
-      <c r="AR14" s="107"/>
-      <c r="AS14" s="108"/>
+      <c r="AR14" s="115"/>
+      <c r="AS14" s="116"/>
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="63"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="65"/>
       <c r="F15" s="8"/>
       <c r="G15" s="54"/>
       <c r="H15" s="9"/>
@@ -2432,21 +2434,21 @@
       <c r="AO15" s="10"/>
       <c r="AP15" s="8"/>
       <c r="AQ15" s="9"/>
-      <c r="AR15" s="107"/>
-      <c r="AS15" s="108"/>
+      <c r="AR15" s="115"/>
+      <c r="AS15" s="116"/>
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="61">
+      <c r="A16" s="77"/>
+      <c r="B16" s="78">
         <v>6</v>
       </c>
-      <c r="C16" s="84" t="s">
+      <c r="C16" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="92">
         <v>2</v>
       </c>
-      <c r="E16" s="118">
+      <c r="E16" s="90">
         <v>2</v>
       </c>
       <c r="F16" s="33"/>
@@ -2487,20 +2489,20 @@
       <c r="AO16" s="10"/>
       <c r="AP16" s="8"/>
       <c r="AQ16" s="9"/>
-      <c r="AR16" s="107"/>
-      <c r="AS16" s="108"/>
+      <c r="AR16" s="115"/>
+      <c r="AS16" s="116"/>
     </row>
     <row r="17" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="74"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="119"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="43"/>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
-      <c r="J17" s="129"/>
+      <c r="J17" s="59"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
@@ -2534,23 +2536,23 @@
       <c r="AO17" s="18"/>
       <c r="AP17" s="16"/>
       <c r="AQ17" s="17"/>
-      <c r="AR17" s="107"/>
-      <c r="AS17" s="108"/>
+      <c r="AR17" s="115"/>
+      <c r="AS17" s="116"/>
     </row>
     <row r="18" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="61">
+      <c r="B18" s="78">
         <v>7</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="116">
+      <c r="D18" s="73">
         <v>2</v>
       </c>
-      <c r="E18" s="117">
+      <c r="E18" s="75">
         <v>2.5</v>
       </c>
       <c r="F18" s="40"/>
@@ -2591,15 +2593,15 @@
       <c r="AO18" s="15"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="7"/>
-      <c r="AR18" s="107"/>
-      <c r="AS18" s="108"/>
+      <c r="AR18" s="115"/>
+      <c r="AS18" s="116"/>
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="65"/>
       <c r="F19" s="33"/>
       <c r="G19" s="28"/>
       <c r="H19" s="54"/>
@@ -2638,21 +2640,21 @@
       <c r="AO19" s="10"/>
       <c r="AP19" s="8"/>
       <c r="AQ19" s="9"/>
-      <c r="AR19" s="107"/>
-      <c r="AS19" s="108"/>
+      <c r="AR19" s="115"/>
+      <c r="AS19" s="116"/>
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="61">
+      <c r="A20" s="77"/>
+      <c r="B20" s="78">
         <v>8</v>
       </c>
-      <c r="C20" s="121" t="s">
+      <c r="C20" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="124">
+      <c r="D20" s="97">
         <v>1</v>
       </c>
-      <c r="E20" s="118">
+      <c r="E20" s="90">
         <v>1</v>
       </c>
       <c r="F20" s="33"/>
@@ -2693,15 +2695,15 @@
       <c r="AO20" s="10"/>
       <c r="AP20" s="8"/>
       <c r="AQ20" s="9"/>
-      <c r="AR20" s="107"/>
-      <c r="AS20" s="108"/>
+      <c r="AR20" s="115"/>
+      <c r="AS20" s="116"/>
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="123"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="96"/>
       <c r="F21" s="33"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2740,21 +2742,21 @@
       <c r="AO21" s="10"/>
       <c r="AP21" s="8"/>
       <c r="AQ21" s="9"/>
-      <c r="AR21" s="107"/>
-      <c r="AS21" s="108"/>
+      <c r="AR21" s="115"/>
+      <c r="AS21" s="116"/>
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="61">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78">
         <v>9</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="62">
+      <c r="D22" s="74">
         <v>1</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="65">
         <v>1</v>
       </c>
       <c r="F22" s="8"/>
@@ -2795,15 +2797,15 @@
       <c r="AO22" s="10"/>
       <c r="AP22" s="8"/>
       <c r="AQ22" s="9"/>
-      <c r="AR22" s="107"/>
-      <c r="AS22" s="108"/>
+      <c r="AR22" s="115"/>
+      <c r="AS22" s="116"/>
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2842,21 +2844,21 @@
       <c r="AO23" s="10"/>
       <c r="AP23" s="8"/>
       <c r="AQ23" s="9"/>
-      <c r="AR23" s="107"/>
-      <c r="AS23" s="108"/>
+      <c r="AR23" s="115"/>
+      <c r="AS23" s="116"/>
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="61">
+      <c r="A24" s="77"/>
+      <c r="B24" s="78">
         <v>10</v>
       </c>
-      <c r="C24" s="64" t="s">
+      <c r="C24" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="74">
         <v>1</v>
       </c>
-      <c r="E24" s="63">
+      <c r="E24" s="65">
         <v>1</v>
       </c>
       <c r="F24" s="8"/>
@@ -2897,15 +2899,15 @@
       <c r="AO24" s="10"/>
       <c r="AP24" s="8"/>
       <c r="AQ24" s="9"/>
-      <c r="AR24" s="107"/>
-      <c r="AS24" s="108"/>
+      <c r="AR24" s="115"/>
+      <c r="AS24" s="116"/>
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="63"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="65"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2944,21 +2946,21 @@
       <c r="AO25" s="10"/>
       <c r="AP25" s="8"/>
       <c r="AQ25" s="9"/>
-      <c r="AR25" s="107"/>
-      <c r="AS25" s="108"/>
+      <c r="AR25" s="115"/>
+      <c r="AS25" s="116"/>
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
-      <c r="B26" s="61">
+      <c r="A26" s="77"/>
+      <c r="B26" s="78">
         <v>11</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="74">
         <v>1</v>
       </c>
-      <c r="E26" s="63">
+      <c r="E26" s="65">
         <v>1</v>
       </c>
       <c r="F26" s="8"/>
@@ -2999,22 +3001,22 @@
       <c r="AO26" s="10"/>
       <c r="AP26" s="8"/>
       <c r="AQ26" s="9"/>
-      <c r="AR26" s="107"/>
-      <c r="AS26" s="108"/>
+      <c r="AR26" s="115"/>
+      <c r="AS26" s="116"/>
     </row>
     <row r="27" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="113"/>
+      <c r="A27" s="79"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
       <c r="I27" s="18"/>
       <c r="J27" s="16"/>
       <c r="K27" s="17"/>
-      <c r="L27" s="131"/>
+      <c r="L27" s="61"/>
       <c r="M27" s="18"/>
       <c r="N27" s="16"/>
       <c r="O27" s="17"/>
@@ -3046,23 +3048,23 @@
       <c r="AO27" s="18"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="17"/>
-      <c r="AR27" s="107"/>
-      <c r="AS27" s="108"/>
+      <c r="AR27" s="115"/>
+      <c r="AS27" s="116"/>
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="126" t="s">
+      <c r="A28" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="61">
+      <c r="B28" s="78">
         <v>12</v>
       </c>
-      <c r="C28" s="115" t="s">
+      <c r="C28" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="116">
+      <c r="D28" s="73">
         <v>1</v>
       </c>
-      <c r="E28" s="117"/>
+      <c r="E28" s="75"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -3101,15 +3103,15 @@
       <c r="AO28" s="15"/>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="7"/>
-      <c r="AR28" s="107"/>
-      <c r="AS28" s="108"/>
+      <c r="AR28" s="115"/>
+      <c r="AS28" s="116"/>
     </row>
     <row r="29" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="127"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="113"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -3117,7 +3119,7 @@
       <c r="J29" s="16"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
-      <c r="M29" s="18"/>
+      <c r="M29" s="62"/>
       <c r="N29" s="16"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
@@ -3148,23 +3150,25 @@
       <c r="AO29" s="18"/>
       <c r="AP29" s="16"/>
       <c r="AQ29" s="17"/>
-      <c r="AR29" s="107"/>
-      <c r="AS29" s="108"/>
+      <c r="AR29" s="115"/>
+      <c r="AS29" s="116"/>
     </row>
     <row r="30" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="61">
+      <c r="B30" s="78">
         <v>13</v>
       </c>
-      <c r="C30" s="128" t="s">
+      <c r="C30" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="116">
+      <c r="D30" s="73">
         <v>2</v>
       </c>
-      <c r="E30" s="117"/>
+      <c r="E30" s="75">
+        <v>1.5</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -3203,15 +3207,15 @@
       <c r="AO30" s="15"/>
       <c r="AP30" s="6"/>
       <c r="AQ30" s="7"/>
-      <c r="AR30" s="107"/>
-      <c r="AS30" s="108"/>
+      <c r="AR30" s="115"/>
+      <c r="AS30" s="116"/>
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="65"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3219,7 +3223,7 @@
       <c r="J31" s="33"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
-      <c r="M31" s="29"/>
+      <c r="M31" s="58"/>
       <c r="N31" s="8"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
@@ -3250,21 +3254,23 @@
       <c r="AO31" s="10"/>
       <c r="AP31" s="8"/>
       <c r="AQ31" s="9"/>
-      <c r="AR31" s="107"/>
-      <c r="AS31" s="108"/>
+      <c r="AR31" s="115"/>
+      <c r="AS31" s="116"/>
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="61">
+      <c r="A32" s="77"/>
+      <c r="B32" s="78">
         <v>14</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="74">
         <v>4</v>
       </c>
-      <c r="E32" s="63"/>
+      <c r="E32" s="65">
+        <v>4</v>
+      </c>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -3303,15 +3309,15 @@
       <c r="AO32" s="10"/>
       <c r="AP32" s="8"/>
       <c r="AQ32" s="9"/>
-      <c r="AR32" s="107"/>
-      <c r="AS32" s="108"/>
+      <c r="AR32" s="115"/>
+      <c r="AS32" s="116"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="65"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3320,8 +3326,8 @@
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="29"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="9"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="54"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="8"/>
@@ -3350,21 +3356,21 @@
       <c r="AO33" s="10"/>
       <c r="AP33" s="8"/>
       <c r="AQ33" s="9"/>
-      <c r="AR33" s="107"/>
-      <c r="AS33" s="108"/>
+      <c r="AR33" s="115"/>
+      <c r="AS33" s="116"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="61">
+      <c r="A34" s="77"/>
+      <c r="B34" s="78">
         <v>15</v>
       </c>
-      <c r="C34" s="65" t="s">
+      <c r="C34" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="74">
         <v>4</v>
       </c>
-      <c r="E34" s="63"/>
+      <c r="E34" s="65"/>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -3403,15 +3409,15 @@
       <c r="AO34" s="10"/>
       <c r="AP34" s="8"/>
       <c r="AQ34" s="9"/>
-      <c r="AR34" s="107"/>
-      <c r="AS34" s="108"/>
+      <c r="AR34" s="115"/>
+      <c r="AS34" s="116"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="63"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="65"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3450,21 +3456,21 @@
       <c r="AO35" s="10"/>
       <c r="AP35" s="8"/>
       <c r="AQ35" s="9"/>
-      <c r="AR35" s="107"/>
-      <c r="AS35" s="108"/>
+      <c r="AR35" s="115"/>
+      <c r="AS35" s="116"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
-      <c r="B36" s="61">
+      <c r="A36" s="77"/>
+      <c r="B36" s="78">
         <v>16</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="62">
+      <c r="D36" s="74">
         <v>2</v>
       </c>
-      <c r="E36" s="63"/>
+      <c r="E36" s="65"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -3503,15 +3509,15 @@
       <c r="AO36" s="10"/>
       <c r="AP36" s="8"/>
       <c r="AQ36" s="9"/>
-      <c r="AR36" s="107"/>
-      <c r="AS36" s="108"/>
+      <c r="AR36" s="115"/>
+      <c r="AS36" s="116"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="63"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="65"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -3550,21 +3556,21 @@
       <c r="AO37" s="10"/>
       <c r="AP37" s="8"/>
       <c r="AQ37" s="9"/>
-      <c r="AR37" s="107"/>
-      <c r="AS37" s="108"/>
+      <c r="AR37" s="115"/>
+      <c r="AS37" s="116"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="73"/>
-      <c r="B38" s="61">
+      <c r="A38" s="77"/>
+      <c r="B38" s="78">
         <v>17</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="68">
+      <c r="D38" s="92">
         <v>2</v>
       </c>
-      <c r="E38" s="63"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -3603,15 +3609,15 @@
       <c r="AO38" s="10"/>
       <c r="AP38" s="8"/>
       <c r="AQ38" s="9"/>
-      <c r="AR38" s="107"/>
-      <c r="AS38" s="108"/>
+      <c r="AR38" s="115"/>
+      <c r="AS38" s="116"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="73"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="63"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="131"/>
+      <c r="D39" s="132"/>
+      <c r="E39" s="65"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -3650,21 +3656,21 @@
       <c r="AO39" s="10"/>
       <c r="AP39" s="8"/>
       <c r="AQ39" s="9"/>
-      <c r="AR39" s="107"/>
-      <c r="AS39" s="108"/>
+      <c r="AR39" s="115"/>
+      <c r="AS39" s="116"/>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="73"/>
-      <c r="B40" s="61">
+      <c r="A40" s="77"/>
+      <c r="B40" s="78">
         <v>18</v>
       </c>
-      <c r="C40" s="65" t="s">
+      <c r="C40" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="62">
+      <c r="D40" s="74">
         <v>2</v>
       </c>
-      <c r="E40" s="63"/>
+      <c r="E40" s="65"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -3703,15 +3709,15 @@
       <c r="AO40" s="10"/>
       <c r="AP40" s="8"/>
       <c r="AQ40" s="9"/>
-      <c r="AR40" s="107"/>
-      <c r="AS40" s="108"/>
+      <c r="AR40" s="115"/>
+      <c r="AS40" s="116"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="73"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="63"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="65"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -3750,21 +3756,21 @@
       <c r="AO41" s="10"/>
       <c r="AP41" s="8"/>
       <c r="AQ41" s="9"/>
-      <c r="AR41" s="107"/>
-      <c r="AS41" s="108"/>
+      <c r="AR41" s="115"/>
+      <c r="AS41" s="116"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="73"/>
-      <c r="B42" s="61">
+      <c r="A42" s="77"/>
+      <c r="B42" s="78">
         <v>19</v>
       </c>
-      <c r="C42" s="75" t="s">
+      <c r="C42" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="62">
+      <c r="D42" s="74">
         <v>1</v>
       </c>
-      <c r="E42" s="63"/>
+      <c r="E42" s="65"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -3803,15 +3809,15 @@
       <c r="AO42" s="10"/>
       <c r="AP42" s="8"/>
       <c r="AQ42" s="9"/>
-      <c r="AR42" s="107"/>
-      <c r="AS42" s="108"/>
+      <c r="AR42" s="115"/>
+      <c r="AS42" s="116"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="73"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="63"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="65"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -3850,21 +3856,21 @@
       <c r="AO43" s="10"/>
       <c r="AP43" s="8"/>
       <c r="AQ43" s="9"/>
-      <c r="AR43" s="107"/>
-      <c r="AS43" s="108"/>
+      <c r="AR43" s="115"/>
+      <c r="AS43" s="116"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="73"/>
-      <c r="B44" s="61">
+      <c r="A44" s="77"/>
+      <c r="B44" s="78">
         <v>20</v>
       </c>
-      <c r="C44" s="75" t="s">
+      <c r="C44" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="62">
+      <c r="D44" s="74">
         <v>1</v>
       </c>
-      <c r="E44" s="63"/>
+      <c r="E44" s="65"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -3903,15 +3909,15 @@
       <c r="AO44" s="10"/>
       <c r="AP44" s="8"/>
       <c r="AQ44" s="9"/>
-      <c r="AR44" s="107"/>
-      <c r="AS44" s="108"/>
+      <c r="AR44" s="115"/>
+      <c r="AS44" s="116"/>
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="73"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -3950,21 +3956,21 @@
       <c r="AO45" s="10"/>
       <c r="AP45" s="8"/>
       <c r="AQ45" s="9"/>
-      <c r="AR45" s="107"/>
-      <c r="AS45" s="108"/>
+      <c r="AR45" s="115"/>
+      <c r="AS45" s="116"/>
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="73"/>
-      <c r="B46" s="61">
+      <c r="A46" s="77"/>
+      <c r="B46" s="78">
         <v>21</v>
       </c>
-      <c r="C46" s="75" t="s">
+      <c r="C46" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="62">
+      <c r="D46" s="74">
         <v>2</v>
       </c>
-      <c r="E46" s="63"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
@@ -4003,15 +4009,15 @@
       <c r="AO46" s="10"/>
       <c r="AP46" s="8"/>
       <c r="AQ46" s="9"/>
-      <c r="AR46" s="107"/>
-      <c r="AS46" s="108"/>
+      <c r="AR46" s="115"/>
+      <c r="AS46" s="116"/>
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="73"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="63"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="65"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4050,21 +4056,21 @@
       <c r="AO47" s="10"/>
       <c r="AP47" s="8"/>
       <c r="AQ47" s="9"/>
-      <c r="AR47" s="107"/>
-      <c r="AS47" s="108"/>
+      <c r="AR47" s="115"/>
+      <c r="AS47" s="116"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="73"/>
-      <c r="B48" s="61">
+      <c r="A48" s="77"/>
+      <c r="B48" s="78">
         <v>22</v>
       </c>
-      <c r="C48" s="77" t="s">
+      <c r="C48" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="79">
+      <c r="D48" s="68">
         <v>2</v>
       </c>
-      <c r="E48" s="63"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -4103,15 +4109,15 @@
       <c r="AO48" s="10"/>
       <c r="AP48" s="8"/>
       <c r="AQ48" s="9"/>
-      <c r="AR48" s="107"/>
-      <c r="AS48" s="108"/>
+      <c r="AR48" s="115"/>
+      <c r="AS48" s="116"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="73"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="63"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -4150,21 +4156,21 @@
       <c r="AO49" s="10"/>
       <c r="AP49" s="8"/>
       <c r="AQ49" s="9"/>
-      <c r="AR49" s="107"/>
-      <c r="AS49" s="108"/>
+      <c r="AR49" s="115"/>
+      <c r="AS49" s="116"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="73"/>
-      <c r="B50" s="61">
+      <c r="A50" s="77"/>
+      <c r="B50" s="78">
         <v>23</v>
       </c>
-      <c r="C50" s="77" t="s">
+      <c r="C50" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="79">
+      <c r="D50" s="68">
         <v>1</v>
       </c>
-      <c r="E50" s="63"/>
+      <c r="E50" s="65"/>
       <c r="F50" s="8"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -4203,15 +4209,15 @@
       <c r="AO50" s="10"/>
       <c r="AP50" s="8"/>
       <c r="AQ50" s="9"/>
-      <c r="AR50" s="107"/>
-      <c r="AS50" s="108"/>
+      <c r="AR50" s="115"/>
+      <c r="AS50" s="116"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="73"/>
-      <c r="B51" s="61"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="63"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="65"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -4250,21 +4256,21 @@
       <c r="AO51" s="10"/>
       <c r="AP51" s="8"/>
       <c r="AQ51" s="9"/>
-      <c r="AR51" s="107"/>
-      <c r="AS51" s="108"/>
+      <c r="AR51" s="115"/>
+      <c r="AS51" s="116"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="73"/>
-      <c r="B52" s="61">
+      <c r="A52" s="77"/>
+      <c r="B52" s="78">
         <v>24</v>
       </c>
-      <c r="C52" s="77" t="s">
+      <c r="C52" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="79">
+      <c r="D52" s="68">
         <v>1</v>
       </c>
-      <c r="E52" s="63"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="8"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -4303,15 +4309,15 @@
       <c r="AO52" s="10"/>
       <c r="AP52" s="8"/>
       <c r="AQ52" s="9"/>
-      <c r="AR52" s="107"/>
-      <c r="AS52" s="108"/>
+      <c r="AR52" s="115"/>
+      <c r="AS52" s="116"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="73"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="63"/>
+      <c r="A53" s="77"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="65"/>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
@@ -4350,21 +4356,21 @@
       <c r="AO53" s="10"/>
       <c r="AP53" s="8"/>
       <c r="AQ53" s="9"/>
-      <c r="AR53" s="107"/>
-      <c r="AS53" s="108"/>
+      <c r="AR53" s="115"/>
+      <c r="AS53" s="116"/>
     </row>
     <row r="54" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="73"/>
-      <c r="B54" s="61">
+      <c r="A54" s="77"/>
+      <c r="B54" s="78">
         <v>25</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="62">
+      <c r="D54" s="74">
         <v>2</v>
       </c>
-      <c r="E54" s="63"/>
+      <c r="E54" s="65"/>
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -4402,15 +4408,15 @@
       <c r="AO54" s="10"/>
       <c r="AP54" s="8"/>
       <c r="AQ54" s="9"/>
-      <c r="AR54" s="107"/>
-      <c r="AS54" s="108"/>
+      <c r="AR54" s="115"/>
+      <c r="AS54" s="116"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="73"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="62"/>
-      <c r="E55" s="63"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="78"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="65"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -4449,21 +4455,21 @@
       <c r="AO55" s="10"/>
       <c r="AP55" s="8"/>
       <c r="AQ55" s="9"/>
-      <c r="AR55" s="107"/>
-      <c r="AS55" s="108"/>
+      <c r="AR55" s="115"/>
+      <c r="AS55" s="116"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="73"/>
-      <c r="B56" s="61">
+      <c r="A56" s="77"/>
+      <c r="B56" s="78">
         <v>26</v>
       </c>
-      <c r="C56" s="75" t="s">
+      <c r="C56" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D56" s="74">
         <v>1</v>
       </c>
-      <c r="E56" s="63"/>
+      <c r="E56" s="65"/>
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
@@ -4502,15 +4508,15 @@
       <c r="AO56" s="10"/>
       <c r="AP56" s="8"/>
       <c r="AQ56" s="9"/>
-      <c r="AR56" s="107"/>
-      <c r="AS56" s="108"/>
+      <c r="AR56" s="115"/>
+      <c r="AS56" s="116"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="73"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="63"/>
+      <c r="A57" s="77"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="65"/>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -4549,21 +4555,21 @@
       <c r="AO57" s="10"/>
       <c r="AP57" s="8"/>
       <c r="AQ57" s="9"/>
-      <c r="AR57" s="107"/>
-      <c r="AS57" s="108"/>
+      <c r="AR57" s="115"/>
+      <c r="AS57" s="116"/>
     </row>
     <row r="58" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
-      <c r="B58" s="61">
+      <c r="A58" s="77"/>
+      <c r="B58" s="78">
         <v>27</v>
       </c>
-      <c r="C58" s="75" t="s">
+      <c r="C58" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D58" s="74">
         <v>1</v>
       </c>
-      <c r="E58" s="63"/>
+      <c r="E58" s="65"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -4602,15 +4608,15 @@
       <c r="AO58" s="10"/>
       <c r="AP58" s="8"/>
       <c r="AQ58" s="9"/>
-      <c r="AR58" s="107"/>
-      <c r="AS58" s="108"/>
+      <c r="AR58" s="115"/>
+      <c r="AS58" s="116"/>
     </row>
     <row r="59" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="73"/>
-      <c r="B59" s="61"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="62"/>
-      <c r="E59" s="63"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="78"/>
+      <c r="C59" s="85"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="65"/>
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
@@ -4649,21 +4655,21 @@
       <c r="AO59" s="10"/>
       <c r="AP59" s="8"/>
       <c r="AQ59" s="9"/>
-      <c r="AR59" s="107"/>
-      <c r="AS59" s="108"/>
+      <c r="AR59" s="115"/>
+      <c r="AS59" s="116"/>
     </row>
     <row r="60" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="73"/>
-      <c r="B60" s="61">
+      <c r="A60" s="77"/>
+      <c r="B60" s="78">
         <v>28</v>
       </c>
-      <c r="C60" s="75" t="s">
+      <c r="C60" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="62">
+      <c r="D60" s="74">
         <v>4</v>
       </c>
-      <c r="E60" s="63"/>
+      <c r="E60" s="65"/>
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
@@ -4702,15 +4708,15 @@
       <c r="AO60" s="10"/>
       <c r="AP60" s="8"/>
       <c r="AQ60" s="9"/>
-      <c r="AR60" s="107"/>
-      <c r="AS60" s="108"/>
+      <c r="AR60" s="115"/>
+      <c r="AS60" s="116"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="73"/>
-      <c r="B61" s="61"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="63"/>
+      <c r="A61" s="77"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="85"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="65"/>
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
@@ -4749,21 +4755,21 @@
       <c r="AO61" s="10"/>
       <c r="AP61" s="8"/>
       <c r="AQ61" s="9"/>
-      <c r="AR61" s="107"/>
-      <c r="AS61" s="108"/>
+      <c r="AR61" s="115"/>
+      <c r="AS61" s="116"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="73"/>
-      <c r="B62" s="61">
+      <c r="A62" s="77"/>
+      <c r="B62" s="78">
         <v>29</v>
       </c>
-      <c r="C62" s="75" t="s">
+      <c r="C62" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="D62" s="62">
+      <c r="D62" s="74">
         <v>2</v>
       </c>
-      <c r="E62" s="63"/>
+      <c r="E62" s="65"/>
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -4802,15 +4808,15 @@
       <c r="AO62" s="10"/>
       <c r="AP62" s="8"/>
       <c r="AQ62" s="9"/>
-      <c r="AR62" s="107"/>
-      <c r="AS62" s="108"/>
+      <c r="AR62" s="115"/>
+      <c r="AS62" s="116"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="73"/>
-      <c r="B63" s="61"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="62"/>
-      <c r="E63" s="63"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="78"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="65"/>
       <c r="F63" s="8"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
@@ -4849,21 +4855,21 @@
       <c r="AO63" s="10"/>
       <c r="AP63" s="8"/>
       <c r="AQ63" s="9"/>
-      <c r="AR63" s="107"/>
-      <c r="AS63" s="108"/>
+      <c r="AR63" s="115"/>
+      <c r="AS63" s="116"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="73"/>
-      <c r="B64" s="61">
+      <c r="A64" s="77"/>
+      <c r="B64" s="78">
         <v>30</v>
       </c>
-      <c r="C64" s="64" t="s">
+      <c r="C64" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="D64" s="62">
+      <c r="D64" s="74">
         <v>2</v>
       </c>
-      <c r="E64" s="63"/>
+      <c r="E64" s="65"/>
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
@@ -4902,15 +4908,15 @@
       <c r="AO64" s="10"/>
       <c r="AP64" s="38"/>
       <c r="AQ64" s="9"/>
-      <c r="AR64" s="107"/>
-      <c r="AS64" s="108"/>
+      <c r="AR64" s="115"/>
+      <c r="AS64" s="116"/>
     </row>
     <row r="65" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="73"/>
-      <c r="B65" s="61"/>
-      <c r="C65" s="64"/>
-      <c r="D65" s="62"/>
-      <c r="E65" s="63"/>
+      <c r="A65" s="77"/>
+      <c r="B65" s="78"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="65"/>
       <c r="F65" s="8"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -4949,23 +4955,23 @@
       <c r="AO65" s="10"/>
       <c r="AP65" s="8"/>
       <c r="AQ65" s="9"/>
-      <c r="AR65" s="107"/>
-      <c r="AS65" s="108"/>
+      <c r="AR65" s="115"/>
+      <c r="AS65" s="116"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="72" t="s">
+      <c r="A66" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="61">
+      <c r="B66" s="78">
         <v>31</v>
       </c>
-      <c r="C66" s="115" t="s">
+      <c r="C66" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="116">
+      <c r="D66" s="73">
         <v>2</v>
       </c>
-      <c r="E66" s="117"/>
+      <c r="E66" s="75"/>
       <c r="F66" s="6"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
@@ -5004,15 +5010,15 @@
       <c r="AO66" s="42"/>
       <c r="AP66" s="6"/>
       <c r="AQ66" s="7"/>
-      <c r="AR66" s="107"/>
-      <c r="AS66" s="108"/>
+      <c r="AR66" s="115"/>
+      <c r="AS66" s="116"/>
     </row>
     <row r="67" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="73"/>
-      <c r="B67" s="61"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="63"/>
+      <c r="A67" s="77"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="65"/>
       <c r="F67" s="8"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
@@ -5051,21 +5057,21 @@
       <c r="AO67" s="29"/>
       <c r="AP67" s="8"/>
       <c r="AQ67" s="9"/>
-      <c r="AR67" s="107"/>
-      <c r="AS67" s="108"/>
+      <c r="AR67" s="115"/>
+      <c r="AS67" s="116"/>
     </row>
     <row r="68" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="73"/>
-      <c r="B68" s="61">
+      <c r="A68" s="77"/>
+      <c r="B68" s="78">
         <v>32</v>
       </c>
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="74">
         <v>4</v>
       </c>
-      <c r="E68" s="63"/>
+      <c r="E68" s="65"/>
       <c r="F68" s="8"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
@@ -5104,15 +5110,15 @@
       <c r="AO68" s="29"/>
       <c r="AP68" s="8"/>
       <c r="AQ68" s="9"/>
-      <c r="AR68" s="107"/>
-      <c r="AS68" s="108"/>
+      <c r="AR68" s="115"/>
+      <c r="AS68" s="116"/>
     </row>
     <row r="69" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="74"/>
-      <c r="B69" s="61"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="112"/>
-      <c r="E69" s="113"/>
+      <c r="A69" s="79"/>
+      <c r="B69" s="78"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="82"/>
       <c r="F69" s="16"/>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
@@ -5151,23 +5157,23 @@
       <c r="AO69" s="45"/>
       <c r="AP69" s="16"/>
       <c r="AQ69" s="17"/>
-      <c r="AR69" s="107"/>
-      <c r="AS69" s="108"/>
+      <c r="AR69" s="115"/>
+      <c r="AS69" s="116"/>
     </row>
     <row r="70" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="72" t="s">
+      <c r="A70" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="61">
+      <c r="B70" s="78">
         <v>33</v>
       </c>
-      <c r="C70" s="64" t="s">
+      <c r="C70" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="62">
+      <c r="D70" s="74">
         <v>1</v>
       </c>
-      <c r="E70" s="63"/>
+      <c r="E70" s="65"/>
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
@@ -5206,15 +5212,15 @@
       <c r="AO70" s="10"/>
       <c r="AP70" s="8"/>
       <c r="AQ70" s="9"/>
-      <c r="AR70" s="107"/>
-      <c r="AS70" s="108"/>
+      <c r="AR70" s="115"/>
+      <c r="AS70" s="116"/>
     </row>
     <row r="71" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="73"/>
-      <c r="B71" s="61"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="62"/>
-      <c r="E71" s="63"/>
+      <c r="A71" s="77"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="65"/>
       <c r="F71" s="8"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
@@ -5253,21 +5259,21 @@
       <c r="AO71" s="10"/>
       <c r="AP71" s="8"/>
       <c r="AQ71" s="9"/>
-      <c r="AR71" s="107"/>
-      <c r="AS71" s="108"/>
+      <c r="AR71" s="115"/>
+      <c r="AS71" s="116"/>
     </row>
     <row r="72" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="73"/>
-      <c r="B72" s="61">
+      <c r="A72" s="77"/>
+      <c r="B72" s="78">
         <v>34</v>
       </c>
-      <c r="C72" s="64" t="s">
+      <c r="C72" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="62">
+      <c r="D72" s="74">
         <v>1</v>
       </c>
-      <c r="E72" s="63"/>
+      <c r="E72" s="65"/>
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
@@ -5306,15 +5312,15 @@
       <c r="AO72" s="10"/>
       <c r="AP72" s="8"/>
       <c r="AQ72" s="9"/>
-      <c r="AR72" s="107"/>
-      <c r="AS72" s="108"/>
+      <c r="AR72" s="115"/>
+      <c r="AS72" s="116"/>
     </row>
     <row r="73" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="73"/>
-      <c r="B73" s="61"/>
-      <c r="C73" s="64"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="63"/>
+      <c r="A73" s="77"/>
+      <c r="B73" s="78"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="65"/>
       <c r="F73" s="8"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
@@ -5353,21 +5359,21 @@
       <c r="AO73" s="10"/>
       <c r="AP73" s="8"/>
       <c r="AQ73" s="9"/>
-      <c r="AR73" s="107"/>
-      <c r="AS73" s="108"/>
+      <c r="AR73" s="115"/>
+      <c r="AS73" s="116"/>
     </row>
     <row r="74" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="73"/>
-      <c r="B74" s="61">
+      <c r="A74" s="77"/>
+      <c r="B74" s="78">
         <v>35</v>
       </c>
-      <c r="C74" s="64" t="s">
+      <c r="C74" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="62">
+      <c r="D74" s="74">
         <v>1</v>
       </c>
-      <c r="E74" s="63"/>
+      <c r="E74" s="65"/>
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
@@ -5406,15 +5412,15 @@
       <c r="AO74" s="10"/>
       <c r="AP74" s="8"/>
       <c r="AQ74" s="9"/>
-      <c r="AR74" s="107"/>
-      <c r="AS74" s="108"/>
+      <c r="AR74" s="115"/>
+      <c r="AS74" s="116"/>
     </row>
     <row r="75" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="73"/>
-      <c r="B75" s="61"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="62"/>
-      <c r="E75" s="63"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="78"/>
+      <c r="C75" s="80"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="65"/>
       <c r="F75" s="8"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
@@ -5453,21 +5459,21 @@
       <c r="AO75" s="10"/>
       <c r="AP75" s="8"/>
       <c r="AQ75" s="9"/>
-      <c r="AR75" s="107"/>
-      <c r="AS75" s="108"/>
+      <c r="AR75" s="115"/>
+      <c r="AS75" s="116"/>
     </row>
     <row r="76" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="73"/>
-      <c r="B76" s="61">
+      <c r="A76" s="77"/>
+      <c r="B76" s="78">
         <v>36</v>
       </c>
-      <c r="C76" s="64" t="s">
+      <c r="C76" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D76" s="62">
+      <c r="D76" s="74">
         <v>1</v>
       </c>
-      <c r="E76" s="63"/>
+      <c r="E76" s="65"/>
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
@@ -5506,15 +5512,15 @@
       <c r="AO76" s="10"/>
       <c r="AP76" s="33"/>
       <c r="AQ76" s="28"/>
-      <c r="AR76" s="107"/>
-      <c r="AS76" s="108"/>
+      <c r="AR76" s="115"/>
+      <c r="AS76" s="116"/>
     </row>
     <row r="77" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="73"/>
-      <c r="B77" s="61"/>
-      <c r="C77" s="64"/>
-      <c r="D77" s="62"/>
-      <c r="E77" s="63"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="78"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="65"/>
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
@@ -5553,21 +5559,21 @@
       <c r="AO77" s="10"/>
       <c r="AP77" s="8"/>
       <c r="AQ77" s="9"/>
-      <c r="AR77" s="107"/>
-      <c r="AS77" s="108"/>
+      <c r="AR77" s="115"/>
+      <c r="AS77" s="116"/>
     </row>
     <row r="78" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="73"/>
-      <c r="B78" s="61">
+      <c r="A78" s="77"/>
+      <c r="B78" s="78">
         <v>37</v>
       </c>
-      <c r="C78" s="64" t="s">
+      <c r="C78" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="62">
+      <c r="D78" s="74">
         <v>1</v>
       </c>
-      <c r="E78" s="63"/>
+      <c r="E78" s="65"/>
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
@@ -5606,15 +5612,15 @@
       <c r="AO78" s="29"/>
       <c r="AP78" s="33"/>
       <c r="AQ78" s="28"/>
-      <c r="AR78" s="107"/>
-      <c r="AS78" s="108"/>
+      <c r="AR78" s="115"/>
+      <c r="AS78" s="116"/>
     </row>
     <row r="79" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="74"/>
-      <c r="B79" s="61"/>
-      <c r="C79" s="111"/>
-      <c r="D79" s="112"/>
-      <c r="E79" s="113"/>
+      <c r="A79" s="79"/>
+      <c r="B79" s="78"/>
+      <c r="C79" s="84"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="82"/>
       <c r="F79" s="16"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
@@ -5653,8 +5659,8 @@
       <c r="AO79" s="45"/>
       <c r="AP79" s="16"/>
       <c r="AQ79" s="17"/>
-      <c r="AR79" s="109"/>
-      <c r="AS79" s="110"/>
+      <c r="AR79" s="117"/>
+      <c r="AS79" s="118"/>
     </row>
     <row r="80" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="51"/>
@@ -5667,63 +5673,230 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>12</v>
+        <v>17.5</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="71" t="s">
+      <c r="A83" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="71"/>
+      <c r="B83" s="133"/>
       <c r="C83" s="50"/>
     </row>
     <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="70" t="s">
+      <c r="A85" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="70"/>
+      <c r="B85" s="64"/>
       <c r="C85" s="23"/>
     </row>
     <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="70" t="s">
+      <c r="A86" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="70"/>
+      <c r="B86" s="64"/>
       <c r="C86" s="24"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="70" t="s">
+      <c r="A87" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="70"/>
+      <c r="B87" s="64"/>
       <c r="C87" s="11"/>
     </row>
     <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="70" t="s">
+      <c r="A88" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B88" s="70"/>
+      <c r="B88" s="64"/>
       <c r="C88" s="57"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="70" t="s">
+      <c r="A90" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B90" s="70"/>
+      <c r="B90" s="64"/>
       <c r="C90" s="48"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="59" t="s">
+      <c r="A91" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="B91" s="60"/>
+      <c r="B91" s="130"/>
       <c r="C91" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="191">
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="A70:A79"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="AR4:AS79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="C44:C45"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="C50:C51"/>
@@ -5748,173 +5921,6 @@
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="AR4:AS79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="A70:A79"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="59" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
updated zeitplan arbeitspaket 16
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11AF24F-93E2-49AA-A418-0A621DEDFEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2704AF-E81A-402C-BD03-1E8F786565C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,11 +1011,59 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1026,6 +1074,144 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1034,192 +1220,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1534,8 +1534,8 @@
   </sheetPr>
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,151 +1552,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="86" t="s">
+      <c r="E1" s="106"/>
+      <c r="F1" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="86" t="s">
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="86" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="86" t="s">
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="86" t="s">
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="86" t="s">
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="86" t="s">
+      <c r="AA1" s="85"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="86" t="s">
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="87"/>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="86" t="s">
+      <c r="AI1" s="85"/>
+      <c r="AJ1" s="85"/>
+      <c r="AK1" s="86"/>
+      <c r="AL1" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="87"/>
-      <c r="AN1" s="87"/>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="101" t="s">
+      <c r="AM1" s="85"/>
+      <c r="AN1" s="85"/>
+      <c r="AO1" s="86"/>
+      <c r="AP1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="AQ1" s="102"/>
-      <c r="AR1" s="102"/>
-      <c r="AS1" s="103"/>
+      <c r="AQ1" s="100"/>
+      <c r="AR1" s="100"/>
+      <c r="AS1" s="101"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A2" s="125"/>
-      <c r="B2" s="122"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="98">
+      <c r="A2" s="94"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="96">
         <v>45351</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="98">
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="96">
         <v>45355</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="98">
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="96">
         <v>45356</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="98">
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="96">
         <v>45357</v>
       </c>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="98">
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="96">
         <v>45358</v>
       </c>
-      <c r="W2" s="99"/>
-      <c r="X2" s="99"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="98">
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="96">
         <v>45362</v>
       </c>
-      <c r="AA2" s="99"/>
-      <c r="AB2" s="99"/>
-      <c r="AC2" s="100"/>
-      <c r="AD2" s="98">
+      <c r="AA2" s="97"/>
+      <c r="AB2" s="97"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="96">
         <v>45363</v>
       </c>
-      <c r="AE2" s="99"/>
-      <c r="AF2" s="99"/>
-      <c r="AG2" s="100"/>
-      <c r="AH2" s="98">
+      <c r="AE2" s="97"/>
+      <c r="AF2" s="97"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="96">
         <v>45364</v>
       </c>
-      <c r="AI2" s="99"/>
-      <c r="AJ2" s="99"/>
-      <c r="AK2" s="100"/>
-      <c r="AL2" s="98">
+      <c r="AI2" s="97"/>
+      <c r="AJ2" s="97"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="96">
         <v>45365</v>
       </c>
-      <c r="AM2" s="99"/>
-      <c r="AN2" s="99"/>
-      <c r="AO2" s="100"/>
-      <c r="AP2" s="98">
+      <c r="AM2" s="97"/>
+      <c r="AN2" s="97"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="96">
         <v>45369</v>
       </c>
-      <c r="AQ2" s="99"/>
-      <c r="AR2" s="99"/>
-      <c r="AS2" s="100"/>
+      <c r="AQ2" s="97"/>
+      <c r="AR2" s="97"/>
+      <c r="AS2" s="98"/>
     </row>
     <row r="3" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126"/>
-      <c r="B3" s="123"/>
-      <c r="C3" s="107"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1825,17 +1825,17 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="119"/>
-      <c r="B4" s="77">
+      <c r="A4" s="87"/>
+      <c r="B4" s="65">
         <v>0</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="66">
         <v>25</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -1874,17 +1874,17 @@
       <c r="AO4" s="26"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="25"/>
-      <c r="AR4" s="112" t="s">
+      <c r="AR4" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="AS4" s="113"/>
+      <c r="AS4" s="110"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="64"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
       <c r="F5" s="52"/>
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
@@ -1923,21 +1923,21 @@
       <c r="AO5" s="29"/>
       <c r="AP5" s="32"/>
       <c r="AQ5" s="28"/>
-      <c r="AR5" s="114"/>
-      <c r="AS5" s="115"/>
+      <c r="AR5" s="111"/>
+      <c r="AS5" s="112"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77">
+      <c r="A6" s="77"/>
+      <c r="B6" s="65">
         <v>1</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="66">
         <v>1</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="67">
         <v>1</v>
       </c>
       <c r="F6" s="37"/>
@@ -1978,15 +1978,15 @@
       <c r="AO6" s="10"/>
       <c r="AP6" s="8"/>
       <c r="AQ6" s="9"/>
-      <c r="AR6" s="114"/>
-      <c r="AS6" s="115"/>
+      <c r="AR6" s="111"/>
+      <c r="AS6" s="112"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="64"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
       <c r="F7" s="52"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -2025,21 +2025,21 @@
       <c r="AO7" s="10"/>
       <c r="AP7" s="8"/>
       <c r="AQ7" s="9"/>
-      <c r="AR7" s="114"/>
-      <c r="AS7" s="115"/>
+      <c r="AR7" s="111"/>
+      <c r="AS7" s="112"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="77">
+      <c r="A8" s="77"/>
+      <c r="B8" s="65">
         <v>2</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="66">
         <v>2</v>
       </c>
-      <c r="E8" s="64"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="32"/>
       <c r="G8" s="28"/>
       <c r="H8" s="9"/>
@@ -2078,15 +2078,15 @@
       <c r="AO8" s="10"/>
       <c r="AP8" s="32"/>
       <c r="AQ8" s="36"/>
-      <c r="AR8" s="114"/>
-      <c r="AS8" s="115"/>
+      <c r="AR8" s="111"/>
+      <c r="AS8" s="112"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="64"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="32"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2125,21 +2125,21 @@
       <c r="AO9" s="10"/>
       <c r="AP9" s="8"/>
       <c r="AQ9" s="9"/>
-      <c r="AR9" s="114"/>
-      <c r="AS9" s="115"/>
+      <c r="AR9" s="111"/>
+      <c r="AS9" s="112"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="77">
+      <c r="A10" s="77"/>
+      <c r="B10" s="65">
         <v>3</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="66">
         <v>1</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="67">
         <v>0.5</v>
       </c>
       <c r="F10" s="8"/>
@@ -2180,14 +2180,14 @@
       <c r="AO10" s="54"/>
       <c r="AP10" s="8"/>
       <c r="AQ10" s="9"/>
-      <c r="AR10" s="114"/>
-      <c r="AS10" s="115"/>
+      <c r="AR10" s="111"/>
+      <c r="AS10" s="112"/>
     </row>
     <row r="11" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="78"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="91"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="118"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
@@ -2227,23 +2227,23 @@
       <c r="AO11" s="14"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="13"/>
-      <c r="AR11" s="114"/>
-      <c r="AS11" s="115"/>
+      <c r="AR11" s="111"/>
+      <c r="AS11" s="112"/>
     </row>
     <row r="12" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="65">
         <v>4</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="72">
+      <c r="D12" s="120">
         <v>1</v>
       </c>
-      <c r="E12" s="74">
+      <c r="E12" s="121">
         <v>1</v>
       </c>
       <c r="F12" s="39"/>
@@ -2284,15 +2284,15 @@
       <c r="AO12" s="15"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="7"/>
-      <c r="AR12" s="114"/>
-      <c r="AS12" s="115"/>
+      <c r="AR12" s="111"/>
+      <c r="AS12" s="112"/>
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="64"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="32"/>
       <c r="G13" s="53"/>
       <c r="H13" s="28"/>
@@ -2331,21 +2331,21 @@
       <c r="AO13" s="10"/>
       <c r="AP13" s="8"/>
       <c r="AQ13" s="9"/>
-      <c r="AR13" s="114"/>
-      <c r="AS13" s="115"/>
+      <c r="AR13" s="111"/>
+      <c r="AS13" s="112"/>
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="77">
+      <c r="A14" s="77"/>
+      <c r="B14" s="65">
         <v>5</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="66">
         <v>1</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="67">
         <v>1</v>
       </c>
       <c r="F14" s="8"/>
@@ -2386,15 +2386,15 @@
       <c r="AO14" s="10"/>
       <c r="AP14" s="8"/>
       <c r="AQ14" s="9"/>
-      <c r="AR14" s="114"/>
-      <c r="AS14" s="115"/>
+      <c r="AR14" s="111"/>
+      <c r="AS14" s="112"/>
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="64"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="8"/>
       <c r="G15" s="53"/>
       <c r="H15" s="9"/>
@@ -2433,21 +2433,21 @@
       <c r="AO15" s="10"/>
       <c r="AP15" s="8"/>
       <c r="AQ15" s="9"/>
-      <c r="AR15" s="114"/>
-      <c r="AS15" s="115"/>
+      <c r="AR15" s="111"/>
+      <c r="AS15" s="112"/>
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77">
+      <c r="A16" s="77"/>
+      <c r="B16" s="65">
         <v>6</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="91">
+      <c r="D16" s="72">
         <v>2</v>
       </c>
-      <c r="E16" s="89">
+      <c r="E16" s="122">
         <v>2</v>
       </c>
       <c r="F16" s="32"/>
@@ -2488,15 +2488,15 @@
       <c r="AO16" s="10"/>
       <c r="AP16" s="8"/>
       <c r="AQ16" s="9"/>
-      <c r="AR16" s="114"/>
-      <c r="AS16" s="115"/>
+      <c r="AR16" s="111"/>
+      <c r="AS16" s="112"/>
     </row>
     <row r="17" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="90"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="123"/>
       <c r="F17" s="42"/>
       <c r="G17" s="43"/>
       <c r="H17" s="43"/>
@@ -2535,23 +2535,23 @@
       <c r="AO17" s="18"/>
       <c r="AP17" s="16"/>
       <c r="AQ17" s="17"/>
-      <c r="AR17" s="114"/>
-      <c r="AS17" s="115"/>
+      <c r="AR17" s="111"/>
+      <c r="AS17" s="112"/>
     </row>
     <row r="18" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="77">
+      <c r="B18" s="65">
         <v>7</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="120">
         <v>2</v>
       </c>
-      <c r="E18" s="74">
+      <c r="E18" s="121">
         <v>2.5</v>
       </c>
       <c r="F18" s="39"/>
@@ -2592,15 +2592,15 @@
       <c r="AO18" s="15"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="7"/>
-      <c r="AR18" s="114"/>
-      <c r="AS18" s="115"/>
+      <c r="AR18" s="111"/>
+      <c r="AS18" s="112"/>
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="64"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="32"/>
       <c r="G19" s="28"/>
       <c r="H19" s="53"/>
@@ -2639,21 +2639,21 @@
       <c r="AO19" s="10"/>
       <c r="AP19" s="8"/>
       <c r="AQ19" s="9"/>
-      <c r="AR19" s="114"/>
-      <c r="AS19" s="115"/>
+      <c r="AR19" s="111"/>
+      <c r="AS19" s="112"/>
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77">
+      <c r="A20" s="77"/>
+      <c r="B20" s="65">
         <v>8</v>
       </c>
-      <c r="C20" s="93" t="s">
+      <c r="C20" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="128">
         <v>1</v>
       </c>
-      <c r="E20" s="89">
+      <c r="E20" s="122">
         <v>1</v>
       </c>
       <c r="F20" s="32"/>
@@ -2694,15 +2694,15 @@
       <c r="AO20" s="10"/>
       <c r="AP20" s="8"/>
       <c r="AQ20" s="9"/>
-      <c r="AR20" s="114"/>
-      <c r="AS20" s="115"/>
+      <c r="AR20" s="111"/>
+      <c r="AS20" s="112"/>
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="95"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="127"/>
       <c r="F21" s="32"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2741,21 +2741,21 @@
       <c r="AO21" s="10"/>
       <c r="AP21" s="8"/>
       <c r="AQ21" s="9"/>
-      <c r="AR21" s="114"/>
-      <c r="AS21" s="115"/>
+      <c r="AR21" s="111"/>
+      <c r="AS21" s="112"/>
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77">
+      <c r="A22" s="77"/>
+      <c r="B22" s="65">
         <v>9</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="73">
+      <c r="D22" s="66">
         <v>1</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="67">
         <v>1</v>
       </c>
       <c r="F22" s="8"/>
@@ -2796,15 +2796,15 @@
       <c r="AO22" s="10"/>
       <c r="AP22" s="8"/>
       <c r="AQ22" s="9"/>
-      <c r="AR22" s="114"/>
-      <c r="AS22" s="115"/>
+      <c r="AR22" s="111"/>
+      <c r="AS22" s="112"/>
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="76"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="64"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="67"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2843,21 +2843,21 @@
       <c r="AO23" s="10"/>
       <c r="AP23" s="8"/>
       <c r="AQ23" s="9"/>
-      <c r="AR23" s="114"/>
-      <c r="AS23" s="115"/>
+      <c r="AR23" s="111"/>
+      <c r="AS23" s="112"/>
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="76"/>
-      <c r="B24" s="77">
+      <c r="A24" s="77"/>
+      <c r="B24" s="65">
         <v>10</v>
       </c>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D24" s="66">
         <v>1</v>
       </c>
-      <c r="E24" s="64">
+      <c r="E24" s="67">
         <v>1</v>
       </c>
       <c r="F24" s="8"/>
@@ -2898,15 +2898,15 @@
       <c r="AO24" s="10"/>
       <c r="AP24" s="8"/>
       <c r="AQ24" s="9"/>
-      <c r="AR24" s="114"/>
-      <c r="AS24" s="115"/>
+      <c r="AR24" s="111"/>
+      <c r="AS24" s="112"/>
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="76"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="64"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="67"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2945,21 +2945,21 @@
       <c r="AO25" s="10"/>
       <c r="AP25" s="8"/>
       <c r="AQ25" s="9"/>
-      <c r="AR25" s="114"/>
-      <c r="AS25" s="115"/>
+      <c r="AR25" s="111"/>
+      <c r="AS25" s="112"/>
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="76"/>
-      <c r="B26" s="77">
+      <c r="A26" s="77"/>
+      <c r="B26" s="65">
         <v>11</v>
       </c>
-      <c r="C26" s="79" t="s">
+      <c r="C26" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="73">
+      <c r="D26" s="66">
         <v>1</v>
       </c>
-      <c r="E26" s="64">
+      <c r="E26" s="67">
         <v>1</v>
       </c>
       <c r="F26" s="8"/>
@@ -3000,15 +3000,15 @@
       <c r="AO26" s="10"/>
       <c r="AP26" s="8"/>
       <c r="AQ26" s="9"/>
-      <c r="AR26" s="114"/>
-      <c r="AS26" s="115"/>
+      <c r="AR26" s="111"/>
+      <c r="AS26" s="112"/>
     </row>
     <row r="27" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="78"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="81"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="117"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -3047,23 +3047,23 @@
       <c r="AO27" s="18"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="17"/>
-      <c r="AR27" s="114"/>
-      <c r="AS27" s="115"/>
+      <c r="AR27" s="111"/>
+      <c r="AS27" s="112"/>
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="77">
+      <c r="B28" s="65">
         <v>12</v>
       </c>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="72">
+      <c r="D28" s="120">
         <v>1</v>
       </c>
-      <c r="E28" s="74"/>
+      <c r="E28" s="121"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -3102,15 +3102,15 @@
       <c r="AO28" s="15"/>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="7"/>
-      <c r="AR28" s="114"/>
-      <c r="AS28" s="115"/>
+      <c r="AR28" s="111"/>
+      <c r="AS28" s="112"/>
     </row>
     <row r="29" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="69"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="81"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="117"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -3149,23 +3149,23 @@
       <c r="AO29" s="18"/>
       <c r="AP29" s="16"/>
       <c r="AQ29" s="17"/>
-      <c r="AR29" s="114"/>
-      <c r="AS29" s="115"/>
+      <c r="AR29" s="111"/>
+      <c r="AS29" s="112"/>
     </row>
     <row r="30" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="77">
+      <c r="B30" s="65">
         <v>13</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="72">
+      <c r="D30" s="120">
         <v>2</v>
       </c>
-      <c r="E30" s="74">
+      <c r="E30" s="121">
         <v>1.5</v>
       </c>
       <c r="F30" s="6"/>
@@ -3206,15 +3206,15 @@
       <c r="AO30" s="15"/>
       <c r="AP30" s="6"/>
       <c r="AQ30" s="7"/>
-      <c r="AR30" s="114"/>
-      <c r="AS30" s="115"/>
+      <c r="AR30" s="111"/>
+      <c r="AS30" s="112"/>
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="76"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="64"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="67"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3253,21 +3253,21 @@
       <c r="AO31" s="10"/>
       <c r="AP31" s="8"/>
       <c r="AQ31" s="9"/>
-      <c r="AR31" s="114"/>
-      <c r="AS31" s="115"/>
+      <c r="AR31" s="111"/>
+      <c r="AS31" s="112"/>
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="77">
+      <c r="A32" s="77"/>
+      <c r="B32" s="65">
         <v>14</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="73">
+      <c r="D32" s="66">
         <v>4</v>
       </c>
-      <c r="E32" s="64">
+      <c r="E32" s="67">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3308,15 +3308,15 @@
       <c r="AO32" s="10"/>
       <c r="AP32" s="8"/>
       <c r="AQ32" s="9"/>
-      <c r="AR32" s="114"/>
-      <c r="AS32" s="115"/>
+      <c r="AR32" s="111"/>
+      <c r="AS32" s="112"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="73"/>
-      <c r="E33" s="64"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3355,21 +3355,21 @@
       <c r="AO33" s="10"/>
       <c r="AP33" s="8"/>
       <c r="AQ33" s="9"/>
-      <c r="AR33" s="114"/>
-      <c r="AS33" s="115"/>
+      <c r="AR33" s="111"/>
+      <c r="AS33" s="112"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="77">
+      <c r="A34" s="77"/>
+      <c r="B34" s="65">
         <v>15</v>
       </c>
-      <c r="C34" s="71" t="s">
+      <c r="C34" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="73">
+      <c r="D34" s="66">
         <v>4</v>
       </c>
-      <c r="E34" s="64">
+      <c r="E34" s="67">
         <v>4</v>
       </c>
       <c r="F34" s="8"/>
@@ -3410,15 +3410,15 @@
       <c r="AO34" s="10"/>
       <c r="AP34" s="8"/>
       <c r="AQ34" s="9"/>
-      <c r="AR34" s="114"/>
-      <c r="AS34" s="115"/>
+      <c r="AR34" s="111"/>
+      <c r="AS34" s="112"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="64"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="67"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3457,21 +3457,21 @@
       <c r="AO35" s="10"/>
       <c r="AP35" s="8"/>
       <c r="AQ35" s="9"/>
-      <c r="AR35" s="114"/>
-      <c r="AS35" s="115"/>
+      <c r="AR35" s="111"/>
+      <c r="AS35" s="112"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="77">
+      <c r="A36" s="77"/>
+      <c r="B36" s="65">
         <v>16</v>
       </c>
-      <c r="C36" s="71" t="s">
+      <c r="C36" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="73">
+      <c r="D36" s="66">
         <v>2</v>
       </c>
-      <c r="E36" s="64"/>
+      <c r="E36" s="67"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -3510,15 +3510,15 @@
       <c r="AO36" s="10"/>
       <c r="AP36" s="8"/>
       <c r="AQ36" s="9"/>
-      <c r="AR36" s="114"/>
-      <c r="AS36" s="115"/>
+      <c r="AR36" s="111"/>
+      <c r="AS36" s="112"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="127"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="64"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="67"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -3531,7 +3531,7 @@
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="10"/>
-      <c r="R37" s="8"/>
+      <c r="R37" s="52"/>
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
       <c r="U37" s="10"/>
@@ -3557,21 +3557,21 @@
       <c r="AO37" s="10"/>
       <c r="AP37" s="8"/>
       <c r="AQ37" s="9"/>
-      <c r="AR37" s="114"/>
-      <c r="AS37" s="115"/>
+      <c r="AR37" s="111"/>
+      <c r="AS37" s="112"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="77">
+      <c r="A38" s="77"/>
+      <c r="B38" s="65">
         <v>17</v>
       </c>
-      <c r="C38" s="127" t="s">
+      <c r="C38" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="91">
+      <c r="D38" s="72">
         <v>2</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -3610,15 +3610,15 @@
       <c r="AO38" s="10"/>
       <c r="AP38" s="8"/>
       <c r="AQ38" s="9"/>
-      <c r="AR38" s="114"/>
-      <c r="AS38" s="115"/>
+      <c r="AR38" s="111"/>
+      <c r="AS38" s="112"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="76"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="130"/>
-      <c r="D39" s="131"/>
-      <c r="E39" s="64"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -3657,21 +3657,21 @@
       <c r="AO39" s="10"/>
       <c r="AP39" s="8"/>
       <c r="AQ39" s="9"/>
-      <c r="AR39" s="114"/>
-      <c r="AS39" s="115"/>
+      <c r="AR39" s="111"/>
+      <c r="AS39" s="112"/>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="77">
+      <c r="A40" s="77"/>
+      <c r="B40" s="65">
         <v>18</v>
       </c>
-      <c r="C40" s="71" t="s">
+      <c r="C40" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="73">
+      <c r="D40" s="66">
         <v>2</v>
       </c>
-      <c r="E40" s="64"/>
+      <c r="E40" s="67"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -3710,15 +3710,15 @@
       <c r="AO40" s="10"/>
       <c r="AP40" s="8"/>
       <c r="AQ40" s="9"/>
-      <c r="AR40" s="114"/>
-      <c r="AS40" s="115"/>
+      <c r="AR40" s="111"/>
+      <c r="AS40" s="112"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="76"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="127"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="64"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="67"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -3757,21 +3757,21 @@
       <c r="AO41" s="10"/>
       <c r="AP41" s="8"/>
       <c r="AQ41" s="9"/>
-      <c r="AR41" s="114"/>
-      <c r="AS41" s="115"/>
+      <c r="AR41" s="111"/>
+      <c r="AS41" s="112"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
-      <c r="B42" s="77">
+      <c r="A42" s="77"/>
+      <c r="B42" s="65">
         <v>19</v>
       </c>
-      <c r="C42" s="84" t="s">
+      <c r="C42" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="73">
+      <c r="D42" s="66">
         <v>1</v>
       </c>
-      <c r="E42" s="64"/>
+      <c r="E42" s="67"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
@@ -3810,15 +3810,15 @@
       <c r="AO42" s="10"/>
       <c r="AP42" s="8"/>
       <c r="AQ42" s="9"/>
-      <c r="AR42" s="114"/>
-      <c r="AS42" s="115"/>
+      <c r="AR42" s="111"/>
+      <c r="AS42" s="112"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="76"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="64"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="65"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="67"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -3857,21 +3857,21 @@
       <c r="AO43" s="10"/>
       <c r="AP43" s="8"/>
       <c r="AQ43" s="9"/>
-      <c r="AR43" s="114"/>
-      <c r="AS43" s="115"/>
+      <c r="AR43" s="111"/>
+      <c r="AS43" s="112"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
-      <c r="B44" s="77">
+      <c r="A44" s="77"/>
+      <c r="B44" s="65">
         <v>20</v>
       </c>
-      <c r="C44" s="84" t="s">
+      <c r="C44" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="73">
+      <c r="D44" s="66">
         <v>1</v>
       </c>
-      <c r="E44" s="64"/>
+      <c r="E44" s="67"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -3910,15 +3910,15 @@
       <c r="AO44" s="10"/>
       <c r="AP44" s="8"/>
       <c r="AQ44" s="9"/>
-      <c r="AR44" s="114"/>
-      <c r="AS44" s="115"/>
+      <c r="AR44" s="111"/>
+      <c r="AS44" s="112"/>
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="76"/>
-      <c r="B45" s="77"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="64"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="67"/>
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -3957,21 +3957,21 @@
       <c r="AO45" s="10"/>
       <c r="AP45" s="8"/>
       <c r="AQ45" s="9"/>
-      <c r="AR45" s="114"/>
-      <c r="AS45" s="115"/>
+      <c r="AR45" s="111"/>
+      <c r="AS45" s="112"/>
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="76"/>
-      <c r="B46" s="77">
+      <c r="A46" s="77"/>
+      <c r="B46" s="65">
         <v>21</v>
       </c>
-      <c r="C46" s="84" t="s">
+      <c r="C46" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="73">
+      <c r="D46" s="66">
         <v>2</v>
       </c>
-      <c r="E46" s="64"/>
+      <c r="E46" s="67"/>
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
@@ -4010,15 +4010,15 @@
       <c r="AO46" s="10"/>
       <c r="AP46" s="8"/>
       <c r="AQ46" s="9"/>
-      <c r="AR46" s="114"/>
-      <c r="AS46" s="115"/>
+      <c r="AR46" s="111"/>
+      <c r="AS46" s="112"/>
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="76"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="64"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4057,21 +4057,21 @@
       <c r="AO47" s="10"/>
       <c r="AP47" s="8"/>
       <c r="AQ47" s="9"/>
-      <c r="AR47" s="114"/>
-      <c r="AS47" s="115"/>
+      <c r="AR47" s="111"/>
+      <c r="AS47" s="112"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="77">
+      <c r="A48" s="77"/>
+      <c r="B48" s="65">
         <v>22</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="67">
+      <c r="D48" s="83">
         <v>2</v>
       </c>
-      <c r="E48" s="64"/>
+      <c r="E48" s="67"/>
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
@@ -4110,15 +4110,15 @@
       <c r="AO48" s="10"/>
       <c r="AP48" s="8"/>
       <c r="AQ48" s="9"/>
-      <c r="AR48" s="114"/>
-      <c r="AS48" s="115"/>
+      <c r="AR48" s="111"/>
+      <c r="AS48" s="112"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="76"/>
-      <c r="B49" s="77"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="64"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="67"/>
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -4157,21 +4157,21 @@
       <c r="AO49" s="10"/>
       <c r="AP49" s="8"/>
       <c r="AQ49" s="9"/>
-      <c r="AR49" s="114"/>
-      <c r="AS49" s="115"/>
+      <c r="AR49" s="111"/>
+      <c r="AS49" s="112"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="76"/>
-      <c r="B50" s="77">
+      <c r="A50" s="77"/>
+      <c r="B50" s="65">
         <v>23</v>
       </c>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="67">
+      <c r="D50" s="83">
         <v>1</v>
       </c>
-      <c r="E50" s="64"/>
+      <c r="E50" s="67"/>
       <c r="F50" s="8"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -4210,15 +4210,15 @@
       <c r="AO50" s="10"/>
       <c r="AP50" s="8"/>
       <c r="AQ50" s="9"/>
-      <c r="AR50" s="114"/>
-      <c r="AS50" s="115"/>
+      <c r="AR50" s="111"/>
+      <c r="AS50" s="112"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="76"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="64"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="67"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -4257,21 +4257,21 @@
       <c r="AO51" s="10"/>
       <c r="AP51" s="8"/>
       <c r="AQ51" s="9"/>
-      <c r="AR51" s="114"/>
-      <c r="AS51" s="115"/>
+      <c r="AR51" s="111"/>
+      <c r="AS51" s="112"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="76"/>
-      <c r="B52" s="77">
+      <c r="A52" s="77"/>
+      <c r="B52" s="65">
         <v>24</v>
       </c>
-      <c r="C52" s="65" t="s">
+      <c r="C52" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="67">
+      <c r="D52" s="83">
         <v>1</v>
       </c>
-      <c r="E52" s="64"/>
+      <c r="E52" s="67"/>
       <c r="F52" s="8"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
@@ -4310,15 +4310,15 @@
       <c r="AO52" s="10"/>
       <c r="AP52" s="8"/>
       <c r="AQ52" s="9"/>
-      <c r="AR52" s="114"/>
-      <c r="AS52" s="115"/>
+      <c r="AR52" s="111"/>
+      <c r="AS52" s="112"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="76"/>
-      <c r="B53" s="77"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="64"/>
+      <c r="A53" s="77"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="67"/>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
@@ -4357,21 +4357,21 @@
       <c r="AO53" s="10"/>
       <c r="AP53" s="8"/>
       <c r="AQ53" s="9"/>
-      <c r="AR53" s="114"/>
-      <c r="AS53" s="115"/>
+      <c r="AR53" s="111"/>
+      <c r="AS53" s="112"/>
     </row>
     <row r="54" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
-      <c r="B54" s="77">
+      <c r="A54" s="77"/>
+      <c r="B54" s="65">
         <v>25</v>
       </c>
-      <c r="C54" s="84" t="s">
+      <c r="C54" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="73">
+      <c r="D54" s="66">
         <v>2</v>
       </c>
-      <c r="E54" s="64"/>
+      <c r="E54" s="67"/>
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -4409,15 +4409,15 @@
       <c r="AO54" s="10"/>
       <c r="AP54" s="8"/>
       <c r="AQ54" s="9"/>
-      <c r="AR54" s="114"/>
-      <c r="AS54" s="115"/>
+      <c r="AR54" s="111"/>
+      <c r="AS54" s="112"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="77"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="64"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="67"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -4456,21 +4456,21 @@
       <c r="AO55" s="10"/>
       <c r="AP55" s="8"/>
       <c r="AQ55" s="9"/>
-      <c r="AR55" s="114"/>
-      <c r="AS55" s="115"/>
+      <c r="AR55" s="111"/>
+      <c r="AS55" s="112"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="76"/>
-      <c r="B56" s="77">
+      <c r="A56" s="77"/>
+      <c r="B56" s="65">
         <v>26</v>
       </c>
-      <c r="C56" s="84" t="s">
+      <c r="C56" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="73">
+      <c r="D56" s="66">
         <v>1</v>
       </c>
-      <c r="E56" s="64"/>
+      <c r="E56" s="67"/>
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
@@ -4509,15 +4509,15 @@
       <c r="AO56" s="10"/>
       <c r="AP56" s="8"/>
       <c r="AQ56" s="9"/>
-      <c r="AR56" s="114"/>
-      <c r="AS56" s="115"/>
+      <c r="AR56" s="111"/>
+      <c r="AS56" s="112"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="76"/>
-      <c r="B57" s="77"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="64"/>
+      <c r="A57" s="77"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="67"/>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -4556,21 +4556,21 @@
       <c r="AO57" s="10"/>
       <c r="AP57" s="8"/>
       <c r="AQ57" s="9"/>
-      <c r="AR57" s="114"/>
-      <c r="AS57" s="115"/>
+      <c r="AR57" s="111"/>
+      <c r="AS57" s="112"/>
     </row>
     <row r="58" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="76"/>
-      <c r="B58" s="77">
+      <c r="A58" s="77"/>
+      <c r="B58" s="65">
         <v>27</v>
       </c>
-      <c r="C58" s="84" t="s">
+      <c r="C58" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="73">
+      <c r="D58" s="66">
         <v>1</v>
       </c>
-      <c r="E58" s="64"/>
+      <c r="E58" s="67"/>
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
@@ -4609,15 +4609,15 @@
       <c r="AO58" s="10"/>
       <c r="AP58" s="8"/>
       <c r="AQ58" s="9"/>
-      <c r="AR58" s="114"/>
-      <c r="AS58" s="115"/>
+      <c r="AR58" s="111"/>
+      <c r="AS58" s="112"/>
     </row>
     <row r="59" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="76"/>
-      <c r="B59" s="77"/>
-      <c r="C59" s="84"/>
-      <c r="D59" s="73"/>
-      <c r="E59" s="64"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="67"/>
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
@@ -4656,21 +4656,21 @@
       <c r="AO59" s="10"/>
       <c r="AP59" s="8"/>
       <c r="AQ59" s="9"/>
-      <c r="AR59" s="114"/>
-      <c r="AS59" s="115"/>
+      <c r="AR59" s="111"/>
+      <c r="AS59" s="112"/>
     </row>
     <row r="60" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="76"/>
-      <c r="B60" s="77">
+      <c r="A60" s="77"/>
+      <c r="B60" s="65">
         <v>28</v>
       </c>
-      <c r="C60" s="84" t="s">
+      <c r="C60" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="73">
+      <c r="D60" s="66">
         <v>4</v>
       </c>
-      <c r="E60" s="64"/>
+      <c r="E60" s="67"/>
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
@@ -4709,15 +4709,15 @@
       <c r="AO60" s="10"/>
       <c r="AP60" s="8"/>
       <c r="AQ60" s="9"/>
-      <c r="AR60" s="114"/>
-      <c r="AS60" s="115"/>
+      <c r="AR60" s="111"/>
+      <c r="AS60" s="112"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="76"/>
-      <c r="B61" s="77"/>
-      <c r="C61" s="84"/>
-      <c r="D61" s="73"/>
-      <c r="E61" s="64"/>
+      <c r="A61" s="77"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="79"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="67"/>
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
@@ -4756,21 +4756,21 @@
       <c r="AO61" s="10"/>
       <c r="AP61" s="8"/>
       <c r="AQ61" s="9"/>
-      <c r="AR61" s="114"/>
-      <c r="AS61" s="115"/>
+      <c r="AR61" s="111"/>
+      <c r="AS61" s="112"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="76"/>
-      <c r="B62" s="77">
+      <c r="A62" s="77"/>
+      <c r="B62" s="65">
         <v>29</v>
       </c>
-      <c r="C62" s="84" t="s">
+      <c r="C62" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="D62" s="73">
+      <c r="D62" s="66">
         <v>2</v>
       </c>
-      <c r="E62" s="64"/>
+      <c r="E62" s="67"/>
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -4809,15 +4809,15 @@
       <c r="AO62" s="10"/>
       <c r="AP62" s="8"/>
       <c r="AQ62" s="9"/>
-      <c r="AR62" s="114"/>
-      <c r="AS62" s="115"/>
+      <c r="AR62" s="111"/>
+      <c r="AS62" s="112"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="76"/>
-      <c r="B63" s="77"/>
-      <c r="C63" s="84"/>
-      <c r="D63" s="73"/>
-      <c r="E63" s="64"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="79"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="67"/>
       <c r="F63" s="8"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
@@ -4856,21 +4856,21 @@
       <c r="AO63" s="10"/>
       <c r="AP63" s="8"/>
       <c r="AQ63" s="9"/>
-      <c r="AR63" s="114"/>
-      <c r="AS63" s="115"/>
+      <c r="AR63" s="111"/>
+      <c r="AS63" s="112"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="76"/>
-      <c r="B64" s="77">
+      <c r="A64" s="77"/>
+      <c r="B64" s="65">
         <v>30</v>
       </c>
-      <c r="C64" s="79" t="s">
+      <c r="C64" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D64" s="73">
+      <c r="D64" s="66">
         <v>2</v>
       </c>
-      <c r="E64" s="64"/>
+      <c r="E64" s="67"/>
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
@@ -4909,15 +4909,15 @@
       <c r="AO64" s="10"/>
       <c r="AP64" s="37"/>
       <c r="AQ64" s="9"/>
-      <c r="AR64" s="114"/>
-      <c r="AS64" s="115"/>
+      <c r="AR64" s="111"/>
+      <c r="AS64" s="112"/>
     </row>
     <row r="65" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="76"/>
-      <c r="B65" s="77"/>
-      <c r="C65" s="79"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="64"/>
+      <c r="A65" s="77"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="67"/>
       <c r="F65" s="8"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -4956,23 +4956,23 @@
       <c r="AO65" s="10"/>
       <c r="AP65" s="8"/>
       <c r="AQ65" s="9"/>
-      <c r="AR65" s="114"/>
-      <c r="AS65" s="115"/>
+      <c r="AR65" s="111"/>
+      <c r="AS65" s="112"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="75" t="s">
+      <c r="A66" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="77">
+      <c r="B66" s="65">
         <v>31</v>
       </c>
-      <c r="C66" s="82" t="s">
+      <c r="C66" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="72">
+      <c r="D66" s="120">
         <v>2</v>
       </c>
-      <c r="E66" s="74"/>
+      <c r="E66" s="121"/>
       <c r="F66" s="6"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
@@ -5011,15 +5011,15 @@
       <c r="AO66" s="41"/>
       <c r="AP66" s="6"/>
       <c r="AQ66" s="7"/>
-      <c r="AR66" s="114"/>
-      <c r="AS66" s="115"/>
+      <c r="AR66" s="111"/>
+      <c r="AS66" s="112"/>
     </row>
     <row r="67" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="76"/>
-      <c r="B67" s="77"/>
-      <c r="C67" s="79"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="64"/>
+      <c r="A67" s="77"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="67"/>
       <c r="F67" s="8"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
@@ -5058,21 +5058,21 @@
       <c r="AO67" s="29"/>
       <c r="AP67" s="8"/>
       <c r="AQ67" s="9"/>
-      <c r="AR67" s="114"/>
-      <c r="AS67" s="115"/>
+      <c r="AR67" s="111"/>
+      <c r="AS67" s="112"/>
     </row>
     <row r="68" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="76"/>
-      <c r="B68" s="77">
+      <c r="A68" s="77"/>
+      <c r="B68" s="65">
         <v>32</v>
       </c>
-      <c r="C68" s="79" t="s">
+      <c r="C68" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="73">
+      <c r="D68" s="66">
         <v>4</v>
       </c>
-      <c r="E68" s="64"/>
+      <c r="E68" s="67"/>
       <c r="F68" s="8"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
@@ -5111,15 +5111,15 @@
       <c r="AO68" s="29"/>
       <c r="AP68" s="8"/>
       <c r="AQ68" s="9"/>
-      <c r="AR68" s="114"/>
-      <c r="AS68" s="115"/>
+      <c r="AR68" s="111"/>
+      <c r="AS68" s="112"/>
     </row>
     <row r="69" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="78"/>
-      <c r="B69" s="77"/>
-      <c r="C69" s="83"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="81"/>
+      <c r="B69" s="65"/>
+      <c r="C69" s="115"/>
+      <c r="D69" s="116"/>
+      <c r="E69" s="117"/>
       <c r="F69" s="16"/>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
@@ -5158,23 +5158,23 @@
       <c r="AO69" s="44"/>
       <c r="AP69" s="16"/>
       <c r="AQ69" s="17"/>
-      <c r="AR69" s="114"/>
-      <c r="AS69" s="115"/>
+      <c r="AR69" s="111"/>
+      <c r="AS69" s="112"/>
     </row>
     <row r="70" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="75" t="s">
+      <c r="A70" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="77">
+      <c r="B70" s="65">
         <v>33</v>
       </c>
-      <c r="C70" s="79" t="s">
+      <c r="C70" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="73">
+      <c r="D70" s="66">
         <v>1</v>
       </c>
-      <c r="E70" s="64"/>
+      <c r="E70" s="67"/>
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
@@ -5213,15 +5213,15 @@
       <c r="AO70" s="10"/>
       <c r="AP70" s="8"/>
       <c r="AQ70" s="9"/>
-      <c r="AR70" s="114"/>
-      <c r="AS70" s="115"/>
+      <c r="AR70" s="111"/>
+      <c r="AS70" s="112"/>
     </row>
     <row r="71" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="76"/>
-      <c r="B71" s="77"/>
-      <c r="C71" s="79"/>
-      <c r="D71" s="73"/>
-      <c r="E71" s="64"/>
+      <c r="A71" s="77"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="67"/>
       <c r="F71" s="8"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
@@ -5260,21 +5260,21 @@
       <c r="AO71" s="10"/>
       <c r="AP71" s="8"/>
       <c r="AQ71" s="9"/>
-      <c r="AR71" s="114"/>
-      <c r="AS71" s="115"/>
+      <c r="AR71" s="111"/>
+      <c r="AS71" s="112"/>
     </row>
     <row r="72" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="76"/>
-      <c r="B72" s="77">
+      <c r="A72" s="77"/>
+      <c r="B72" s="65">
         <v>34</v>
       </c>
-      <c r="C72" s="79" t="s">
+      <c r="C72" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="73">
+      <c r="D72" s="66">
         <v>1</v>
       </c>
-      <c r="E72" s="64"/>
+      <c r="E72" s="67"/>
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
@@ -5313,15 +5313,15 @@
       <c r="AO72" s="10"/>
       <c r="AP72" s="8"/>
       <c r="AQ72" s="9"/>
-      <c r="AR72" s="114"/>
-      <c r="AS72" s="115"/>
+      <c r="AR72" s="111"/>
+      <c r="AS72" s="112"/>
     </row>
     <row r="73" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="76"/>
-      <c r="B73" s="77"/>
-      <c r="C73" s="79"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="64"/>
+      <c r="A73" s="77"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="67"/>
       <c r="F73" s="8"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
@@ -5360,21 +5360,21 @@
       <c r="AO73" s="10"/>
       <c r="AP73" s="8"/>
       <c r="AQ73" s="9"/>
-      <c r="AR73" s="114"/>
-      <c r="AS73" s="115"/>
+      <c r="AR73" s="111"/>
+      <c r="AS73" s="112"/>
     </row>
     <row r="74" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="76"/>
-      <c r="B74" s="77">
+      <c r="A74" s="77"/>
+      <c r="B74" s="65">
         <v>35</v>
       </c>
-      <c r="C74" s="79" t="s">
+      <c r="C74" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="73">
+      <c r="D74" s="66">
         <v>1</v>
       </c>
-      <c r="E74" s="64"/>
+      <c r="E74" s="67"/>
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
@@ -5413,15 +5413,15 @@
       <c r="AO74" s="10"/>
       <c r="AP74" s="8"/>
       <c r="AQ74" s="9"/>
-      <c r="AR74" s="114"/>
-      <c r="AS74" s="115"/>
+      <c r="AR74" s="111"/>
+      <c r="AS74" s="112"/>
     </row>
     <row r="75" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="76"/>
-      <c r="B75" s="77"/>
-      <c r="C75" s="79"/>
-      <c r="D75" s="73"/>
-      <c r="E75" s="64"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="67"/>
       <c r="F75" s="8"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
@@ -5460,21 +5460,21 @@
       <c r="AO75" s="10"/>
       <c r="AP75" s="8"/>
       <c r="AQ75" s="9"/>
-      <c r="AR75" s="114"/>
-      <c r="AS75" s="115"/>
+      <c r="AR75" s="111"/>
+      <c r="AS75" s="112"/>
     </row>
     <row r="76" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="76"/>
-      <c r="B76" s="77">
+      <c r="A76" s="77"/>
+      <c r="B76" s="65">
         <v>36</v>
       </c>
-      <c r="C76" s="79" t="s">
+      <c r="C76" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D76" s="73">
+      <c r="D76" s="66">
         <v>1</v>
       </c>
-      <c r="E76" s="64"/>
+      <c r="E76" s="67"/>
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
@@ -5513,15 +5513,15 @@
       <c r="AO76" s="10"/>
       <c r="AP76" s="32"/>
       <c r="AQ76" s="28"/>
-      <c r="AR76" s="114"/>
-      <c r="AS76" s="115"/>
+      <c r="AR76" s="111"/>
+      <c r="AS76" s="112"/>
     </row>
     <row r="77" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="76"/>
-      <c r="B77" s="77"/>
-      <c r="C77" s="79"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="64"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="65"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="67"/>
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
@@ -5560,21 +5560,21 @@
       <c r="AO77" s="10"/>
       <c r="AP77" s="8"/>
       <c r="AQ77" s="9"/>
-      <c r="AR77" s="114"/>
-      <c r="AS77" s="115"/>
+      <c r="AR77" s="111"/>
+      <c r="AS77" s="112"/>
     </row>
     <row r="78" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="76"/>
-      <c r="B78" s="77">
+      <c r="A78" s="77"/>
+      <c r="B78" s="65">
         <v>37</v>
       </c>
-      <c r="C78" s="79" t="s">
+      <c r="C78" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="73">
+      <c r="D78" s="66">
         <v>1</v>
       </c>
-      <c r="E78" s="64"/>
+      <c r="E78" s="67"/>
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
@@ -5613,15 +5613,15 @@
       <c r="AO78" s="29"/>
       <c r="AP78" s="32"/>
       <c r="AQ78" s="28"/>
-      <c r="AR78" s="114"/>
-      <c r="AS78" s="115"/>
+      <c r="AR78" s="111"/>
+      <c r="AS78" s="112"/>
     </row>
     <row r="79" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="78"/>
-      <c r="B79" s="77"/>
-      <c r="C79" s="83"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="81"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="115"/>
+      <c r="D79" s="116"/>
+      <c r="E79" s="117"/>
       <c r="F79" s="16"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
@@ -5660,8 +5660,8 @@
       <c r="AO79" s="44"/>
       <c r="AP79" s="16"/>
       <c r="AQ79" s="17"/>
-      <c r="AR79" s="116"/>
-      <c r="AS79" s="117"/>
+      <c r="AR79" s="113"/>
+      <c r="AS79" s="114"/>
     </row>
     <row r="80" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="50"/>
@@ -5681,56 +5681,223 @@
     </row>
     <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="132" t="s">
+      <c r="A83" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="132"/>
+      <c r="B83" s="75"/>
       <c r="C83" s="49"/>
     </row>
     <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="63" t="s">
+      <c r="A85" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="63"/>
+      <c r="B85" s="74"/>
       <c r="C85" s="23"/>
     </row>
     <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="63" t="s">
+      <c r="A86" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="63"/>
+      <c r="B86" s="74"/>
       <c r="C86" s="24"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="63" t="s">
+      <c r="A87" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="63"/>
+      <c r="B87" s="74"/>
       <c r="C87" s="11"/>
     </row>
     <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="63" t="s">
+      <c r="A88" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B88" s="63"/>
+      <c r="B88" s="74"/>
       <c r="C88" s="56"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="63" t="s">
+      <c r="A90" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B90" s="63"/>
+      <c r="B90" s="74"/>
       <c r="C90" s="47"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="128" t="s">
+      <c r="A91" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B91" s="129"/>
+      <c r="B91" s="64"/>
       <c r="C91" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="191">
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A30:A65"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="AR4:AS79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="A70:A79"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
@@ -5755,173 +5922,6 @@
     <mergeCell ref="B70:B71"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="A70:A79"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="AR4:AS79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A30:A65"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A18:A27"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="59" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
updated zeitplam arbeitspaket 17
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96808F13-8DDC-42FB-BF19-A21CB1CBFCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7C40BC-1DB5-4033-A006-F0FFDBB083B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1535,7 +1535,7 @@
   <dimension ref="A1:AS91"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3573,7 +3573,9 @@
       <c r="D38" s="72">
         <v>2</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="67">
+        <v>2</v>
+      </c>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -3634,7 +3636,7 @@
       <c r="P39" s="28"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="8"/>
-      <c r="S39" s="9"/>
+      <c r="S39" s="53"/>
       <c r="T39" s="9"/>
       <c r="U39" s="10"/>
       <c r="V39" s="8"/>
@@ -5676,7 +5678,7 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>

</xml_diff>

<commit_message>
updated zeitplan day 4
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7C40BC-1DB5-4033-A006-F0FFDBB083B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01378A9E-D88E-4FAF-82FD-A5FB9455A865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,8 +1534,8 @@
   </sheetPr>
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,8 +1899,8 @@
       <c r="Q5" s="62"/>
       <c r="R5" s="32"/>
       <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="29"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="57"/>
       <c r="V5" s="32"/>
       <c r="W5" s="28"/>
       <c r="X5" s="28"/>
@@ -3063,7 +3063,9 @@
       <c r="D28" s="120">
         <v>1</v>
       </c>
-      <c r="E28" s="121"/>
+      <c r="E28" s="121">
+        <v>1</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -3675,7 +3677,9 @@
       <c r="D40" s="66">
         <v>2</v>
       </c>
-      <c r="E40" s="67"/>
+      <c r="E40" s="67">
+        <v>3</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
@@ -3737,7 +3741,7 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="32"/>
       <c r="S41" s="28"/>
-      <c r="T41" s="28"/>
+      <c r="T41" s="53"/>
       <c r="U41" s="29"/>
       <c r="V41" s="32"/>
       <c r="W41" s="28"/>
@@ -5678,7 +5682,7 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>25.5</v>
+        <v>29.5</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>

</xml_diff>

<commit_message>
updated zeitplan, finished day 5
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD28084-0380-46D2-A83E-E34F3B98337E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F85051-2151-4BB2-AD01-EC36FE831D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,8 +1534,8 @@
   </sheetPr>
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated zeitplan, finished arbeitspaket 29 and meilenstein 3
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46C9A7-37E5-49B6-8980-022264617A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A0E796-F51D-4A24-B3EE-8F30D24AEF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,8 +1534,8 @@
   </sheetPr>
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF63" sqref="AF63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,7 +4798,9 @@
       <c r="D62" s="66">
         <v>2</v>
       </c>
-      <c r="E62" s="67"/>
+      <c r="E62" s="67">
+        <v>3</v>
+      </c>
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -4872,7 +4874,7 @@
       <c r="AC63" s="29"/>
       <c r="AD63" s="8"/>
       <c r="AE63" s="9"/>
-      <c r="AF63" s="9"/>
+      <c r="AF63" s="53"/>
       <c r="AG63" s="10"/>
       <c r="AH63" s="8"/>
       <c r="AI63" s="9"/>
@@ -5702,7 +5704,7 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>

</xml_diff>

<commit_message>
updated Zeitplan day 8
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7697D29-795B-44FA-B560-8DEDB20B4050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E917A4EA-59D2-4A6E-9711-D7B0DB482D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,8 +1534,8 @@
   </sheetPr>
   <dimension ref="A1:AS91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AU18" sqref="AU18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AV67" sqref="AV67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,8 +1915,8 @@
       <c r="AG5" s="57"/>
       <c r="AH5" s="52"/>
       <c r="AI5" s="53"/>
-      <c r="AJ5" s="28"/>
-      <c r="AK5" s="29"/>
+      <c r="AJ5" s="53"/>
+      <c r="AK5" s="57"/>
       <c r="AL5" s="32"/>
       <c r="AM5" s="28"/>
       <c r="AN5" s="28"/>
@@ -5182,8 +5182,8 @@
       <c r="AG69" s="18"/>
       <c r="AH69" s="42"/>
       <c r="AI69" s="43"/>
-      <c r="AJ69" s="43"/>
-      <c r="AK69" s="44"/>
+      <c r="AJ69" s="60"/>
+      <c r="AK69" s="61"/>
       <c r="AL69" s="42"/>
       <c r="AM69" s="43"/>
       <c r="AN69" s="43"/>

</xml_diff>

<commit_message>
added auswertung teilauftrag 1
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A0AC0A-3582-468F-A89B-2328FCC57170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C8EA0-563E-49E8-AF96-241F68875684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>Aufwand (h)</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Expertenbesuch</t>
+  </si>
+  <si>
+    <t>Die Zahlen im Zeitplan markieren jeweils das Ende eines Arbeitsintervalls: „10“ steht für 10 Uhr, das Ende des ersten Blocks, der um 8 Uhr beginnt.</t>
+  </si>
+  <si>
+    <t>Zeitangaben</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -931,11 +937,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1221,6 +1238,10 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1532,10 +1553,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS91"/>
+  <dimension ref="A1:AS93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM69" sqref="AM69"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL33" sqref="AL33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,7 +1941,7 @@
       <c r="AL5" s="52"/>
       <c r="AM5" s="53"/>
       <c r="AN5" s="53"/>
-      <c r="AO5" s="29"/>
+      <c r="AO5" s="57"/>
       <c r="AP5" s="32"/>
       <c r="AQ5" s="28"/>
       <c r="AR5" s="111"/>
@@ -2224,7 +2245,7 @@
       <c r="AL11" s="35"/>
       <c r="AM11" s="33"/>
       <c r="AN11" s="13"/>
-      <c r="AO11" s="14"/>
+      <c r="AO11" s="55"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="13"/>
       <c r="AR11" s="111"/>
@@ -5208,7 +5229,9 @@
       <c r="D70" s="66">
         <v>1</v>
       </c>
-      <c r="E70" s="67"/>
+      <c r="E70" s="67">
+        <v>1</v>
+      </c>
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
@@ -5291,7 +5314,7 @@
       <c r="AL71" s="8"/>
       <c r="AM71" s="9"/>
       <c r="AN71" s="9"/>
-      <c r="AO71" s="10"/>
+      <c r="AO71" s="57"/>
       <c r="AP71" s="8"/>
       <c r="AQ71" s="9"/>
       <c r="AR71" s="111"/>
@@ -5708,60 +5731,85 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="75" t="s">
         <v>56</v>
       </c>
       <c r="B83" s="75"/>
       <c r="C83" s="49"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="74" t="s">
         <v>5</v>
       </c>
       <c r="B85" s="74"/>
       <c r="C85" s="23"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B86" s="74"/>
       <c r="C86" s="24"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="74" t="s">
         <v>9</v>
       </c>
       <c r="B87" s="74"/>
       <c r="C87" s="11"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="74" t="s">
         <v>59</v>
       </c>
       <c r="B88" s="74"/>
       <c r="C88" s="56"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="74" t="s">
         <v>54</v>
       </c>
       <c r="B90" s="74"/>
       <c r="C90" s="47"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="63" t="s">
         <v>55</v>
       </c>
       <c r="B91" s="64"/>
       <c r="C91" s="48"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" s="134"/>
+      <c r="C93" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" s="135"/>
+      <c r="E93" s="135"/>
+      <c r="F93" s="135"/>
+      <c r="G93" s="135"/>
+      <c r="H93" s="135"/>
+      <c r="I93" s="135"/>
+      <c r="J93" s="135"/>
+      <c r="K93" s="135"/>
+      <c r="L93" s="135"/>
+      <c r="M93" s="135"/>
+      <c r="N93" s="135"/>
+      <c r="O93" s="135"/>
+      <c r="P93" s="135"/>
+      <c r="Q93" s="135"/>
+      <c r="R93" s="135"/>
+      <c r="S93" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="191">

</xml_diff>

<commit_message>
updated zeitplan finished deployment
</commit_message>
<xml_diff>
--- a/IPA-Zeitplan.xlsx
+++ b/IPA-Zeitplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C8EA0-563E-49E8-AF96-241F68875684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5449341E-E601-45B3-A315-7D9EFD725820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,220 +1028,220 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1555,8 +1555,8 @@
   </sheetPr>
   <dimension ref="A1:AS93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL33" sqref="AL33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,151 +1573,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="125" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="105" t="s">
+      <c r="D1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="106"/>
-      <c r="F1" s="84" t="s">
+      <c r="E1" s="113"/>
+      <c r="F1" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="84" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="84" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="84" t="s">
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="84" t="s">
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="84" t="s">
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="84" t="s">
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="86"/>
-      <c r="AH1" s="84" t="s">
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="85"/>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="84" t="s">
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="92"/>
+      <c r="AL1" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="85"/>
-      <c r="AN1" s="85"/>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="99" t="s">
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="AQ1" s="100"/>
-      <c r="AR1" s="100"/>
-      <c r="AS1" s="101"/>
+      <c r="AQ1" s="106"/>
+      <c r="AR1" s="106"/>
+      <c r="AS1" s="107"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="96">
+      <c r="A2" s="129"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="102">
         <v>45351</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="96">
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="102">
         <v>45355</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="96">
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="102">
         <v>45356</v>
       </c>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="96">
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="102">
         <v>45357</v>
       </c>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="96">
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="102">
         <v>45358</v>
       </c>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="98"/>
-      <c r="Z2" s="96">
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="102">
         <v>45362</v>
       </c>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="98"/>
-      <c r="AD2" s="96">
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="104"/>
+      <c r="AD2" s="102">
         <v>45363</v>
       </c>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="98"/>
-      <c r="AH2" s="96">
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="104"/>
+      <c r="AH2" s="102">
         <v>45364</v>
       </c>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="98"/>
-      <c r="AL2" s="96">
+      <c r="AI2" s="103"/>
+      <c r="AJ2" s="103"/>
+      <c r="AK2" s="104"/>
+      <c r="AL2" s="102">
         <v>45365</v>
       </c>
-      <c r="AM2" s="97"/>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="98"/>
-      <c r="AP2" s="96">
+      <c r="AM2" s="103"/>
+      <c r="AN2" s="103"/>
+      <c r="AO2" s="104"/>
+      <c r="AP2" s="102">
         <v>45369</v>
       </c>
-      <c r="AQ2" s="97"/>
-      <c r="AR2" s="97"/>
-      <c r="AS2" s="98"/>
+      <c r="AQ2" s="103"/>
+      <c r="AR2" s="103"/>
+      <c r="AS2" s="104"/>
     </row>
     <row r="3" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="95"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="104"/>
+      <c r="A3" s="130"/>
+      <c r="B3" s="127"/>
+      <c r="C3" s="111"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1846,17 +1846,17 @@
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="65">
+      <c r="A4" s="123"/>
+      <c r="B4" s="81">
         <v>0</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="77">
         <v>25</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -1895,17 +1895,17 @@
       <c r="AO4" s="26"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="25"/>
-      <c r="AR4" s="109" t="s">
+      <c r="AR4" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="AS4" s="110"/>
+      <c r="AS4" s="117"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="52"/>
       <c r="G5" s="53"/>
       <c r="H5" s="53"/>
@@ -1944,21 +1944,21 @@
       <c r="AO5" s="57"/>
       <c r="AP5" s="32"/>
       <c r="AQ5" s="28"/>
-      <c r="AR5" s="111"/>
-      <c r="AS5" s="112"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="119"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
-      <c r="B6" s="65">
+      <c r="A6" s="80"/>
+      <c r="B6" s="81">
         <v>1</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="66">
+      <c r="D6" s="77">
         <v>1</v>
       </c>
-      <c r="E6" s="67">
+      <c r="E6" s="68">
         <v>1</v>
       </c>
       <c r="F6" s="37"/>
@@ -1999,15 +1999,15 @@
       <c r="AO6" s="10"/>
       <c r="AP6" s="8"/>
       <c r="AQ6" s="9"/>
-      <c r="AR6" s="111"/>
-      <c r="AS6" s="112"/>
+      <c r="AR6" s="118"/>
+      <c r="AS6" s="119"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="77"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="52"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -2046,21 +2046,21 @@
       <c r="AO7" s="10"/>
       <c r="AP7" s="8"/>
       <c r="AQ7" s="9"/>
-      <c r="AR7" s="111"/>
-      <c r="AS7" s="112"/>
+      <c r="AR7" s="118"/>
+      <c r="AS7" s="119"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
-      <c r="B8" s="65">
+      <c r="A8" s="80"/>
+      <c r="B8" s="81">
         <v>2</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="77">
         <v>2</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="32"/>
       <c r="G8" s="28"/>
       <c r="H8" s="9"/>
@@ -2099,15 +2099,15 @@
       <c r="AO8" s="10"/>
       <c r="AP8" s="32"/>
       <c r="AQ8" s="36"/>
-      <c r="AR8" s="111"/>
-      <c r="AS8" s="112"/>
+      <c r="AR8" s="118"/>
+      <c r="AS8" s="119"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="32"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2146,21 +2146,21 @@
       <c r="AO9" s="10"/>
       <c r="AP9" s="8"/>
       <c r="AQ9" s="9"/>
-      <c r="AR9" s="111"/>
-      <c r="AS9" s="112"/>
+      <c r="AR9" s="118"/>
+      <c r="AS9" s="119"/>
     </row>
     <row r="10" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
-      <c r="B10" s="65">
+      <c r="A10" s="80"/>
+      <c r="B10" s="81">
         <v>3</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="77">
         <v>1</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="68">
         <v>0.5</v>
       </c>
       <c r="F10" s="8"/>
@@ -2201,15 +2201,15 @@
       <c r="AO10" s="54"/>
       <c r="AP10" s="8"/>
       <c r="AQ10" s="9"/>
-      <c r="AR10" s="111"/>
-      <c r="AS10" s="112"/>
+      <c r="AR10" s="118"/>
+      <c r="AS10" s="119"/>
     </row>
     <row r="11" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="118"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="122"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2248,23 +2248,23 @@
       <c r="AO11" s="55"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="13"/>
-      <c r="AR11" s="111"/>
-      <c r="AS11" s="112"/>
+      <c r="AR11" s="118"/>
+      <c r="AS11" s="119"/>
     </row>
     <row r="12" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="81">
         <v>4</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="120">
+      <c r="D12" s="76">
         <v>1</v>
       </c>
-      <c r="E12" s="121">
+      <c r="E12" s="78">
         <v>1</v>
       </c>
       <c r="F12" s="39"/>
@@ -2305,15 +2305,15 @@
       <c r="AO12" s="15"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="7"/>
-      <c r="AR12" s="111"/>
-      <c r="AS12" s="112"/>
+      <c r="AR12" s="118"/>
+      <c r="AS12" s="119"/>
     </row>
     <row r="13" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="32"/>
       <c r="G13" s="53"/>
       <c r="H13" s="28"/>
@@ -2352,21 +2352,21 @@
       <c r="AO13" s="10"/>
       <c r="AP13" s="8"/>
       <c r="AQ13" s="9"/>
-      <c r="AR13" s="111"/>
-      <c r="AS13" s="112"/>
+      <c r="AR13" s="118"/>
+      <c r="AS13" s="119"/>
     </row>
     <row r="14" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="65">
+      <c r="A14" s="80"/>
+      <c r="B14" s="81">
         <v>5</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="66">
+      <c r="D14" s="77">
         <v>1</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="68">
         <v>1</v>
       </c>
       <c r="F14" s="8"/>
@@ -2407,15 +2407,15 @@
       <c r="AO14" s="10"/>
       <c r="AP14" s="8"/>
       <c r="AQ14" s="9"/>
-      <c r="AR14" s="111"/>
-      <c r="AS14" s="112"/>
+      <c r="AR14" s="118"/>
+      <c r="AS14" s="119"/>
     </row>
     <row r="15" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="77"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="67"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="8"/>
       <c r="G15" s="53"/>
       <c r="H15" s="9"/>
@@ -2454,21 +2454,21 @@
       <c r="AO15" s="10"/>
       <c r="AP15" s="8"/>
       <c r="AQ15" s="9"/>
-      <c r="AR15" s="111"/>
-      <c r="AS15" s="112"/>
+      <c r="AR15" s="118"/>
+      <c r="AS15" s="119"/>
     </row>
     <row r="16" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="65">
+      <c r="A16" s="80"/>
+      <c r="B16" s="81">
         <v>6</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="95">
         <v>2</v>
       </c>
-      <c r="E16" s="122">
+      <c r="E16" s="93">
         <v>2</v>
       </c>
       <c r="F16" s="32"/>
@@ -2509,15 +2509,15 @@
       <c r="AO16" s="10"/>
       <c r="AP16" s="8"/>
       <c r="AQ16" s="9"/>
-      <c r="AR16" s="111"/>
-      <c r="AS16" s="112"/>
+      <c r="AR16" s="118"/>
+      <c r="AS16" s="119"/>
     </row>
     <row r="17" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="78"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="123"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="42"/>
       <c r="G17" s="43"/>
       <c r="H17" s="43"/>
@@ -2556,23 +2556,23 @@
       <c r="AO17" s="18"/>
       <c r="AP17" s="16"/>
       <c r="AQ17" s="17"/>
-      <c r="AR17" s="111"/>
-      <c r="AS17" s="112"/>
+      <c r="AR17" s="118"/>
+      <c r="AS17" s="119"/>
     </row>
     <row r="18" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="81">
         <v>7</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="120">
+      <c r="D18" s="76">
         <v>2</v>
       </c>
-      <c r="E18" s="121">
+      <c r="E18" s="78">
         <v>2.5</v>
       </c>
       <c r="F18" s="39"/>
@@ -2613,15 +2613,15 @@
       <c r="AO18" s="15"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="7"/>
-      <c r="AR18" s="111"/>
-      <c r="AS18" s="112"/>
+      <c r="AR18" s="118"/>
+      <c r="AS18" s="119"/>
     </row>
     <row r="19" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="67"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="32"/>
       <c r="G19" s="28"/>
       <c r="H19" s="53"/>
@@ -2660,21 +2660,21 @@
       <c r="AO19" s="10"/>
       <c r="AP19" s="8"/>
       <c r="AQ19" s="9"/>
-      <c r="AR19" s="111"/>
-      <c r="AS19" s="112"/>
+      <c r="AR19" s="118"/>
+      <c r="AS19" s="119"/>
     </row>
     <row r="20" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="77"/>
-      <c r="B20" s="65">
+      <c r="A20" s="80"/>
+      <c r="B20" s="81">
         <v>8</v>
       </c>
-      <c r="C20" s="125" t="s">
+      <c r="C20" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="128">
+      <c r="D20" s="100">
         <v>1</v>
       </c>
-      <c r="E20" s="122">
+      <c r="E20" s="93">
         <v>1</v>
       </c>
       <c r="F20" s="32"/>
@@ -2715,15 +2715,15 @@
       <c r="AO20" s="10"/>
       <c r="AP20" s="8"/>
       <c r="AQ20" s="9"/>
-      <c r="AR20" s="111"/>
-      <c r="AS20" s="112"/>
+      <c r="AR20" s="118"/>
+      <c r="AS20" s="119"/>
     </row>
     <row r="21" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="126"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="127"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="99"/>
       <c r="F21" s="32"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2762,21 +2762,21 @@
       <c r="AO21" s="10"/>
       <c r="AP21" s="8"/>
       <c r="AQ21" s="9"/>
-      <c r="AR21" s="111"/>
-      <c r="AS21" s="112"/>
+      <c r="AR21" s="118"/>
+      <c r="AS21" s="119"/>
     </row>
     <row r="22" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="77"/>
-      <c r="B22" s="65">
+      <c r="A22" s="80"/>
+      <c r="B22" s="81">
         <v>9</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="66">
+      <c r="D22" s="77">
         <v>1</v>
       </c>
-      <c r="E22" s="67">
+      <c r="E22" s="68">
         <v>1</v>
       </c>
       <c r="F22" s="8"/>
@@ -2817,15 +2817,15 @@
       <c r="AO22" s="10"/>
       <c r="AP22" s="8"/>
       <c r="AQ22" s="9"/>
-      <c r="AR22" s="111"/>
-      <c r="AS22" s="112"/>
+      <c r="AR22" s="118"/>
+      <c r="AS22" s="119"/>
     </row>
     <row r="23" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="67"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="68"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2864,21 +2864,21 @@
       <c r="AO23" s="10"/>
       <c r="AP23" s="8"/>
       <c r="AQ23" s="9"/>
-      <c r="AR23" s="111"/>
-      <c r="AS23" s="112"/>
+      <c r="AR23" s="118"/>
+      <c r="AS23" s="119"/>
     </row>
     <row r="24" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="65">
+      <c r="A24" s="80"/>
+      <c r="B24" s="81">
         <v>10</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="66">
+      <c r="D24" s="77">
         <v>1</v>
       </c>
-      <c r="E24" s="67">
+      <c r="E24" s="68">
         <v>1</v>
       </c>
       <c r="F24" s="8"/>
@@ -2919,15 +2919,15 @@
       <c r="AO24" s="10"/>
       <c r="AP24" s="8"/>
       <c r="AQ24" s="9"/>
-      <c r="AR24" s="111"/>
-      <c r="AS24" s="112"/>
+      <c r="AR24" s="118"/>
+      <c r="AS24" s="119"/>
     </row>
     <row r="25" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="67"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="68"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2966,21 +2966,21 @@
       <c r="AO25" s="10"/>
       <c r="AP25" s="8"/>
       <c r="AQ25" s="9"/>
-      <c r="AR25" s="111"/>
-      <c r="AS25" s="112"/>
+      <c r="AR25" s="118"/>
+      <c r="AS25" s="119"/>
     </row>
     <row r="26" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
-      <c r="B26" s="65">
+      <c r="A26" s="80"/>
+      <c r="B26" s="81">
         <v>11</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="77">
         <v>1</v>
       </c>
-      <c r="E26" s="67">
+      <c r="E26" s="68">
         <v>1</v>
       </c>
       <c r="F26" s="8"/>
@@ -3021,15 +3021,15 @@
       <c r="AO26" s="10"/>
       <c r="AP26" s="8"/>
       <c r="AQ26" s="9"/>
-      <c r="AR26" s="111"/>
-      <c r="AS26" s="112"/>
+      <c r="AR26" s="118"/>
+      <c r="AS26" s="119"/>
     </row>
     <row r="27" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="115"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="117"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="85"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -3068,23 +3068,23 @@
       <c r="AO27" s="18"/>
       <c r="AP27" s="16"/>
       <c r="AQ27" s="17"/>
-      <c r="AR27" s="111"/>
-      <c r="AS27" s="112"/>
+      <c r="AR27" s="118"/>
+      <c r="AS27" s="119"/>
     </row>
     <row r="28" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="130" t="s">
+      <c r="A28" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="65">
+      <c r="B28" s="81">
         <v>12</v>
       </c>
-      <c r="C28" s="119" t="s">
+      <c r="C28" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="120">
+      <c r="D28" s="76">
         <v>1</v>
       </c>
-      <c r="E28" s="121">
+      <c r="E28" s="78">
         <v>1</v>
       </c>
       <c r="F28" s="6"/>
@@ -3125,15 +3125,15 @@
       <c r="AO28" s="15"/>
       <c r="AP28" s="6"/>
       <c r="AQ28" s="7"/>
-      <c r="AR28" s="111"/>
-      <c r="AS28" s="112"/>
+      <c r="AR28" s="118"/>
+      <c r="AS28" s="119"/>
     </row>
     <row r="29" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="131"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="117"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="85"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -3172,23 +3172,23 @@
       <c r="AO29" s="18"/>
       <c r="AP29" s="16"/>
       <c r="AQ29" s="17"/>
-      <c r="AR29" s="111"/>
-      <c r="AS29" s="112"/>
+      <c r="AR29" s="118"/>
+      <c r="AS29" s="119"/>
     </row>
     <row r="30" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="65">
+      <c r="B30" s="81">
         <v>13</v>
       </c>
-      <c r="C30" s="132" t="s">
+      <c r="C30" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="120">
+      <c r="D30" s="76">
         <v>2</v>
       </c>
-      <c r="E30" s="121">
+      <c r="E30" s="78">
         <v>1.5</v>
       </c>
       <c r="F30" s="6"/>
@@ -3229,15 +3229,15 @@
       <c r="AO30" s="15"/>
       <c r="AP30" s="6"/>
       <c r="AQ30" s="7"/>
-      <c r="AR30" s="111"/>
-      <c r="AS30" s="112"/>
+      <c r="AR30" s="118"/>
+      <c r="AS30" s="119"/>
     </row>
     <row r="31" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="67"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="68"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -3276,21 +3276,21 @@
       <c r="AO31" s="10"/>
       <c r="AP31" s="8"/>
       <c r="AQ31" s="9"/>
-      <c r="AR31" s="111"/>
-      <c r="AS31" s="112"/>
+      <c r="AR31" s="118"/>
+      <c r="AS31" s="119"/>
     </row>
     <row r="32" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
-      <c r="B32" s="65">
+      <c r="A32" s="80"/>
+      <c r="B32" s="81">
         <v>14</v>
       </c>
-      <c r="C32" s="69" t="s">
+      <c r="C32" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="66">
+      <c r="D32" s="77">
         <v>4</v>
       </c>
-      <c r="E32" s="67">
+      <c r="E32" s="68">
         <v>4</v>
       </c>
       <c r="F32" s="8"/>
@@ -3331,15 +3331,15 @@
       <c r="AO32" s="10"/>
       <c r="AP32" s="8"/>
       <c r="AQ32" s="9"/>
-      <c r="AR32" s="111"/>
-      <c r="AS32" s="112"/>
+      <c r="AR32" s="118"/>
+      <c r="AS32" s="119"/>
     </row>
     <row r="33" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="67"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -3378,21 +3378,21 @@
       <c r="AO33" s="10"/>
       <c r="AP33" s="8"/>
       <c r="AQ33" s="9"/>
-      <c r="AR33" s="111"/>
-      <c r="AS33" s="112"/>
+      <c r="AR33" s="118"/>
+      <c r="AS33" s="119"/>
     </row>
     <row r="34" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="65">
+      <c r="A34" s="80"/>
+      <c r="B34" s="81">
         <v>15</v>
       </c>
-      <c r="C34" s="69" t="s">
+      <c r="C34" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="66">
+      <c r="D34" s="77">
         <v>4</v>
       </c>
-      <c r="E34" s="67">
+      <c r="E34" s="68">
         <v>4</v>
       </c>
       <c r="F34" s="8"/>
@@ -3433,15 +3433,15 @@
       <c r="AO34" s="10"/>
       <c r="AP34" s="8"/>
       <c r="AQ34" s="9"/>
-      <c r="AR34" s="111"/>
-      <c r="AS34" s="112"/>
+      <c r="AR34" s="118"/>
+      <c r="AS34" s="119"/>
     </row>
     <row r="35" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="67"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -3480,21 +3480,21 @@
       <c r="AO35" s="10"/>
       <c r="AP35" s="8"/>
       <c r="AQ35" s="9"/>
-      <c r="AR35" s="111"/>
-      <c r="AS35" s="112"/>
+      <c r="AR35" s="118"/>
+      <c r="AS35" s="119"/>
     </row>
     <row r="36" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
-      <c r="B36" s="65">
+      <c r="A36" s="80"/>
+      <c r="B36" s="81">
         <v>16</v>
       </c>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="66">
+      <c r="D36" s="77">
         <v>2</v>
       </c>
-      <c r="E36" s="67">
+      <c r="E36" s="68">
         <v>2</v>
       </c>
       <c r="F36" s="8"/>
@@ -3535,15 +3535,15 @@
       <c r="AO36" s="10"/>
       <c r="AP36" s="8"/>
       <c r="AQ36" s="9"/>
-      <c r="AR36" s="111"/>
-      <c r="AS36" s="112"/>
+      <c r="AR36" s="118"/>
+      <c r="AS36" s="119"/>
     </row>
     <row r="37" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="65"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="67"/>
+      <c r="A37" s="80"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="131"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -3582,21 +3582,21 @@
       <c r="AO37" s="10"/>
       <c r="AP37" s="8"/>
       <c r="AQ37" s="9"/>
-      <c r="AR37" s="111"/>
-      <c r="AS37" s="112"/>
+      <c r="AR37" s="118"/>
+      <c r="AS37" s="119"/>
     </row>
     <row r="38" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="65">
+      <c r="A38" s="80"/>
+      <c r="B38" s="81">
         <v>17</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="72">
+      <c r="D38" s="95">
         <v>2</v>
       </c>
-      <c r="E38" s="67">
+      <c r="E38" s="68">
         <v>2</v>
       </c>
       <c r="F38" s="8"/>
@@ -3637,15 +3637,15 @@
       <c r="AO38" s="10"/>
       <c r="AP38" s="8"/>
       <c r="AQ38" s="9"/>
-      <c r="AR38" s="111"/>
-      <c r="AS38" s="112"/>
+      <c r="AR38" s="118"/>
+      <c r="AS38" s="119"/>
     </row>
     <row r="39" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="67"/>
+      <c r="A39" s="80"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="135"/>
+      <c r="E39" s="68"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
@@ -3684,21 +3684,21 @@
       <c r="AO39" s="10"/>
       <c r="AP39" s="8"/>
       <c r="AQ39" s="9"/>
-      <c r="AR39" s="111"/>
-      <c r="AS39" s="112"/>
+      <c r="AR39" s="118"/>
+      <c r="AS39" s="119"/>
     </row>
     <row r="40" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
-      <c r="B40" s="65">
+      <c r="A40" s="80"/>
+      <c r="B40" s="81">
         <v>18</v>
       </c>
-      <c r="C40" s="69" t="s">
+      <c r="C40" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="66">
+      <c r="D40" s="77">
         <v>2</v>
       </c>
-      <c r="E40" s="67">
+      <c r="E40" s="68">
         <v>3</v>
       </c>
       <c r="F40" s="8"/>
@@ -3739,15 +3739,15 @@
       <c r="AO40" s="10"/>
       <c r="AP40" s="8"/>
       <c r="AQ40" s="9"/>
-      <c r="AR40" s="111"/>
-      <c r="AS40" s="112"/>
+      <c r="AR40" s="118"/>
+      <c r="AS40" s="119"/>
     </row>
     <row r="41" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="67"/>
+      <c r="A41" s="80"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="68"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
@@ -3786,21 +3786,21 @@
       <c r="AO41" s="10"/>
       <c r="AP41" s="8"/>
       <c r="AQ41" s="9"/>
-      <c r="AR41" s="111"/>
-      <c r="AS41" s="112"/>
+      <c r="AR41" s="118"/>
+      <c r="AS41" s="119"/>
     </row>
     <row r="42" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="77"/>
-      <c r="B42" s="65">
+      <c r="A42" s="80"/>
+      <c r="B42" s="81">
         <v>19</v>
       </c>
-      <c r="C42" s="79" t="s">
+      <c r="C42" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="66">
+      <c r="D42" s="77">
         <v>1</v>
       </c>
-      <c r="E42" s="67">
+      <c r="E42" s="68">
         <v>0.5</v>
       </c>
       <c r="F42" s="8"/>
@@ -3841,15 +3841,15 @@
       <c r="AO42" s="10"/>
       <c r="AP42" s="8"/>
       <c r="AQ42" s="9"/>
-      <c r="AR42" s="111"/>
-      <c r="AS42" s="112"/>
+      <c r="AR42" s="118"/>
+      <c r="AS42" s="119"/>
     </row>
     <row r="43" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="77"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="67"/>
+      <c r="A43" s="80"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="68"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
@@ -3888,21 +3888,21 @@
       <c r="AO43" s="10"/>
       <c r="AP43" s="8"/>
       <c r="AQ43" s="9"/>
-      <c r="AR43" s="111"/>
-      <c r="AS43" s="112"/>
+      <c r="AR43" s="118"/>
+      <c r="AS43" s="119"/>
     </row>
     <row r="44" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="77"/>
-      <c r="B44" s="65">
+      <c r="A44" s="80"/>
+      <c r="B44" s="81">
         <v>20</v>
       </c>
-      <c r="C44" s="79" t="s">
+      <c r="C44" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="66">
+      <c r="D44" s="77">
         <v>1</v>
       </c>
-      <c r="E44" s="67">
+      <c r="E44" s="68">
         <v>1</v>
       </c>
       <c r="F44" s="8"/>
@@ -3943,15 +3943,15 @@
       <c r="AO44" s="10"/>
       <c r="AP44" s="8"/>
       <c r="AQ44" s="9"/>
-      <c r="AR44" s="111"/>
-      <c r="AS44" s="112"/>
+      <c r="AR44" s="118"/>
+      <c r="AS44" s="119"/>
     </row>
     <row r="45" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="77"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="67"/>
+      <c r="A45" s="80"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="68"/>
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
@@ -3990,21 +3990,21 @@
       <c r="AO45" s="10"/>
       <c r="AP45" s="8"/>
       <c r="AQ45" s="9"/>
-      <c r="AR45" s="111"/>
-      <c r="AS45" s="112"/>
+      <c r="AR45" s="118"/>
+      <c r="AS45" s="119"/>
     </row>
     <row r="46" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="77"/>
-      <c r="B46" s="65">
+      <c r="A46" s="80"/>
+      <c r="B46" s="81">
         <v>21</v>
       </c>
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="66">
+      <c r="D46" s="77">
         <v>2</v>
       </c>
-      <c r="E46" s="67">
+      <c r="E46" s="68">
         <v>1.5</v>
       </c>
       <c r="F46" s="8"/>
@@ -4045,15 +4045,15 @@
       <c r="AO46" s="10"/>
       <c r="AP46" s="8"/>
       <c r="AQ46" s="9"/>
-      <c r="AR46" s="111"/>
-      <c r="AS46" s="112"/>
+      <c r="AR46" s="118"/>
+      <c r="AS46" s="119"/>
     </row>
     <row r="47" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="77"/>
-      <c r="B47" s="65"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="67"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="68"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
@@ -4092,21 +4092,21 @@
       <c r="AO47" s="10"/>
       <c r="AP47" s="8"/>
       <c r="AQ47" s="9"/>
-      <c r="AR47" s="111"/>
-      <c r="AS47" s="112"/>
+      <c r="AR47" s="118"/>
+      <c r="AS47" s="119"/>
     </row>
     <row r="48" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="77"/>
-      <c r="B48" s="65">
+      <c r="A48" s="80"/>
+      <c r="B48" s="81">
         <v>22</v>
       </c>
-      <c r="C48" s="81" t="s">
+      <c r="C48" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="83">
+      <c r="D48" s="71">
         <v>2</v>
       </c>
-      <c r="E48" s="67">
+      <c r="E48" s="68">
         <v>2</v>
       </c>
       <c r="F48" s="8"/>
@@ -4147,15 +4147,15 @@
       <c r="AO48" s="10"/>
       <c r="AP48" s="8"/>
       <c r="AQ48" s="9"/>
-      <c r="AR48" s="111"/>
-      <c r="AS48" s="112"/>
+      <c r="AR48" s="118"/>
+      <c r="AS48" s="119"/>
     </row>
     <row r="49" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
-      <c r="B49" s="65"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="67"/>
+      <c r="A49" s="80"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="68"/>
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -4194,21 +4194,21 @@
       <c r="AO49" s="10"/>
       <c r="AP49" s="8"/>
       <c r="AQ49" s="9"/>
-      <c r="AR49" s="111"/>
-      <c r="AS49" s="112"/>
+      <c r="AR49" s="118"/>
+      <c r="AS49" s="119"/>
     </row>
     <row r="50" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
-      <c r="B50" s="65">
+      <c r="A50" s="80"/>
+      <c r="B50" s="81">
         <v>23</v>
       </c>
-      <c r="C50" s="81" t="s">
+      <c r="C50" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="83">
+      <c r="D50" s="71">
         <v>1</v>
       </c>
-      <c r="E50" s="67">
+      <c r="E50" s="68">
         <v>1</v>
       </c>
       <c r="F50" s="8"/>
@@ -4249,15 +4249,15 @@
       <c r="AO50" s="10"/>
       <c r="AP50" s="8"/>
       <c r="AQ50" s="9"/>
-      <c r="AR50" s="111"/>
-      <c r="AS50" s="112"/>
+      <c r="AR50" s="118"/>
+      <c r="AS50" s="119"/>
     </row>
     <row r="51" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="77"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="67"/>
+      <c r="A51" s="80"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="68"/>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -4296,21 +4296,21 @@
       <c r="AO51" s="10"/>
       <c r="AP51" s="8"/>
       <c r="AQ51" s="9"/>
-      <c r="AR51" s="111"/>
-      <c r="AS51" s="112"/>
+      <c r="AR51" s="118"/>
+      <c r="AS51" s="119"/>
     </row>
     <row r="52" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="77"/>
-      <c r="B52" s="65">
+      <c r="A52" s="80"/>
+      <c r="B52" s="81">
         <v>24</v>
       </c>
-      <c r="C52" s="81" t="s">
+      <c r="C52" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="83">
+      <c r="D52" s="71">
         <v>1</v>
       </c>
-      <c r="E52" s="67">
+      <c r="E52" s="68">
         <v>1</v>
       </c>
       <c r="F52" s="8"/>
@@ -4351,15 +4351,15 @@
       <c r="AO52" s="10"/>
       <c r="AP52" s="8"/>
       <c r="AQ52" s="9"/>
-      <c r="AR52" s="111"/>
-      <c r="AS52" s="112"/>
+      <c r="AR52" s="118"/>
+      <c r="AS52" s="119"/>
     </row>
     <row r="53" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="77"/>
-      <c r="B53" s="65"/>
-      <c r="C53" s="82"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="67"/>
+      <c r="A53" s="80"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="70"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="68"/>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
@@ -4398,21 +4398,21 @@
       <c r="AO53" s="10"/>
       <c r="AP53" s="8"/>
       <c r="AQ53" s="9"/>
-      <c r="AR53" s="111"/>
-      <c r="AS53" s="112"/>
+      <c r="AR53" s="118"/>
+      <c r="AS53" s="119"/>
     </row>
     <row r="54" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="77"/>
-      <c r="B54" s="65">
+      <c r="A54" s="80"/>
+      <c r="B54" s="81">
         <v>25</v>
       </c>
-      <c r="C54" s="79" t="s">
+      <c r="C54" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="66">
+      <c r="D54" s="77">
         <v>2</v>
       </c>
-      <c r="E54" s="67">
+      <c r="E54" s="68">
         <v>3</v>
       </c>
       <c r="F54" s="8"/>
@@ -4452,15 +4452,15 @@
       <c r="AO54" s="10"/>
       <c r="AP54" s="8"/>
       <c r="AQ54" s="9"/>
-      <c r="AR54" s="111"/>
-      <c r="AS54" s="112"/>
+      <c r="AR54" s="118"/>
+      <c r="AS54" s="119"/>
     </row>
     <row r="55" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="77"/>
-      <c r="B55" s="65"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="67"/>
+      <c r="A55" s="80"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
@@ -4499,21 +4499,21 @@
       <c r="AO55" s="10"/>
       <c r="AP55" s="8"/>
       <c r="AQ55" s="9"/>
-      <c r="AR55" s="111"/>
-      <c r="AS55" s="112"/>
+      <c r="AR55" s="118"/>
+      <c r="AS55" s="119"/>
     </row>
     <row r="56" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="77"/>
-      <c r="B56" s="65">
+      <c r="A56" s="80"/>
+      <c r="B56" s="81">
         <v>26</v>
       </c>
-      <c r="C56" s="79" t="s">
+      <c r="C56" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="66">
+      <c r="D56" s="77">
         <v>1</v>
       </c>
-      <c r="E56" s="67">
+      <c r="E56" s="68">
         <v>1</v>
       </c>
       <c r="F56" s="8"/>
@@ -4554,15 +4554,15 @@
       <c r="AO56" s="10"/>
       <c r="AP56" s="8"/>
       <c r="AQ56" s="9"/>
-      <c r="AR56" s="111"/>
-      <c r="AS56" s="112"/>
+      <c r="AR56" s="118"/>
+      <c r="AS56" s="119"/>
     </row>
     <row r="57" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="77"/>
-      <c r="B57" s="65"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="67"/>
+      <c r="A57" s="80"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="88"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="68"/>
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
@@ -4601,21 +4601,21 @@
       <c r="AO57" s="10"/>
       <c r="AP57" s="8"/>
       <c r="AQ57" s="9"/>
-      <c r="AR57" s="111"/>
-      <c r="AS57" s="112"/>
+      <c r="AR57" s="118"/>
+      <c r="AS57" s="119"/>
     </row>
     <row r="58" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="77"/>
-      <c r="B58" s="65">
+      <c r="A58" s="80"/>
+      <c r="B58" s="81">
         <v>27</v>
       </c>
-      <c r="C58" s="79" t="s">
+      <c r="C58" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="66">
+      <c r="D58" s="77">
         <v>1</v>
       </c>
-      <c r="E58" s="67">
+      <c r="E58" s="68">
         <v>0.5</v>
       </c>
       <c r="F58" s="8"/>
@@ -4656,15 +4656,15 @@
       <c r="AO58" s="10"/>
       <c r="AP58" s="8"/>
       <c r="AQ58" s="9"/>
-      <c r="AR58" s="111"/>
-      <c r="AS58" s="112"/>
+      <c r="AR58" s="118"/>
+      <c r="AS58" s="119"/>
     </row>
     <row r="59" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="77"/>
-      <c r="B59" s="65"/>
-      <c r="C59" s="79"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="67"/>
+      <c r="A59" s="80"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="77"/>
+      <c r="E59" s="68"/>
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
@@ -4703,21 +4703,21 @@
       <c r="AO59" s="10"/>
       <c r="AP59" s="8"/>
       <c r="AQ59" s="9"/>
-      <c r="AR59" s="111"/>
-      <c r="AS59" s="112"/>
+      <c r="AR59" s="118"/>
+      <c r="AS59" s="119"/>
     </row>
     <row r="60" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="77"/>
-      <c r="B60" s="65">
+      <c r="A60" s="80"/>
+      <c r="B60" s="81">
         <v>28</v>
       </c>
-      <c r="C60" s="79" t="s">
+      <c r="C60" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="66">
+      <c r="D60" s="77">
         <v>4</v>
       </c>
-      <c r="E60" s="67">
+      <c r="E60" s="68">
         <v>4</v>
       </c>
       <c r="F60" s="8"/>
@@ -4758,15 +4758,15 @@
       <c r="AO60" s="10"/>
       <c r="AP60" s="8"/>
       <c r="AQ60" s="9"/>
-      <c r="AR60" s="111"/>
-      <c r="AS60" s="112"/>
+      <c r="AR60" s="118"/>
+      <c r="AS60" s="119"/>
     </row>
     <row r="61" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="77"/>
-      <c r="B61" s="65"/>
-      <c r="C61" s="79"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="67"/>
+      <c r="A61" s="80"/>
+      <c r="B61" s="81"/>
+      <c r="C61" s="88"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="68"/>
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
@@ -4805,21 +4805,21 @@
       <c r="AO61" s="10"/>
       <c r="AP61" s="8"/>
       <c r="AQ61" s="9"/>
-      <c r="AR61" s="111"/>
-      <c r="AS61" s="112"/>
+      <c r="AR61" s="118"/>
+      <c r="AS61" s="119"/>
     </row>
     <row r="62" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="77"/>
-      <c r="B62" s="65">
+      <c r="A62" s="80"/>
+      <c r="B62" s="81">
         <v>29</v>
       </c>
-      <c r="C62" s="79" t="s">
+      <c r="C62" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D62" s="66">
+      <c r="D62" s="77">
         <v>2</v>
       </c>
-      <c r="E62" s="67">
+      <c r="E62" s="68">
         <v>3</v>
       </c>
       <c r="F62" s="8"/>
@@ -4860,15 +4860,15 @@
       <c r="AO62" s="10"/>
       <c r="AP62" s="8"/>
       <c r="AQ62" s="9"/>
-      <c r="AR62" s="111"/>
-      <c r="AS62" s="112"/>
+      <c r="AR62" s="118"/>
+      <c r="AS62" s="119"/>
     </row>
     <row r="63" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="77"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="79"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="67"/>
+      <c r="A63" s="80"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="88"/>
+      <c r="D63" s="77"/>
+      <c r="E63" s="68"/>
       <c r="F63" s="8"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
@@ -4907,21 +4907,23 @@
       <c r="AO63" s="10"/>
       <c r="AP63" s="8"/>
       <c r="AQ63" s="9"/>
-      <c r="AR63" s="111"/>
-      <c r="AS63" s="112"/>
+      <c r="AR63" s="118"/>
+      <c r="AS63" s="119"/>
     </row>
     <row r="64" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="77"/>
-      <c r="B64" s="65">
+      <c r="A64" s="80"/>
+      <c r="B64" s="81">
         <v>30</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D64" s="66">
+      <c r="D64" s="77">
         <v>2</v>
       </c>
-      <c r="E64" s="67"/>
+      <c r="E64" s="68">
+        <v>2</v>
+      </c>
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
@@ -4960,15 +4962,15 @@
       <c r="AO64" s="10"/>
       <c r="AP64" s="37"/>
       <c r="AQ64" s="9"/>
-      <c r="AR64" s="111"/>
-      <c r="AS64" s="112"/>
+      <c r="AR64" s="118"/>
+      <c r="AS64" s="119"/>
     </row>
     <row r="65" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="77"/>
-      <c r="B65" s="65"/>
-      <c r="C65" s="68"/>
-      <c r="D65" s="66"/>
-      <c r="E65" s="67"/>
+      <c r="A65" s="80"/>
+      <c r="B65" s="81"/>
+      <c r="C65" s="83"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="68"/>
       <c r="F65" s="8"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -5005,25 +5007,25 @@
       <c r="AM65" s="9"/>
       <c r="AN65" s="9"/>
       <c r="AO65" s="10"/>
-      <c r="AP65" s="8"/>
+      <c r="AP65" s="52"/>
       <c r="AQ65" s="9"/>
-      <c r="AR65" s="111"/>
-      <c r="AS65" s="112"/>
+      <c r="AR65" s="118"/>
+      <c r="AS65" s="119"/>
     </row>
     <row r="66" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="76" t="s">
+      <c r="A66" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="65">
+      <c r="B66" s="81">
         <v>31</v>
       </c>
-      <c r="C66" s="119" t="s">
+      <c r="C66" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="120">
+      <c r="D66" s="76">
         <v>2</v>
       </c>
-      <c r="E66" s="121">
+      <c r="E66" s="78">
         <v>2</v>
       </c>
       <c r="F66" s="6"/>
@@ -5064,15 +5066,15 @@
       <c r="AO66" s="41"/>
       <c r="AP66" s="6"/>
       <c r="AQ66" s="7"/>
-      <c r="AR66" s="111"/>
-      <c r="AS66" s="112"/>
+      <c r="AR66" s="118"/>
+      <c r="AS66" s="119"/>
     </row>
     <row r="67" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="77"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="66"/>
-      <c r="E67" s="67"/>
+      <c r="A67" s="80"/>
+      <c r="B67" s="81"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="68"/>
       <c r="F67" s="8"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
@@ -5111,21 +5113,21 @@
       <c r="AO67" s="29"/>
       <c r="AP67" s="8"/>
       <c r="AQ67" s="9"/>
-      <c r="AR67" s="111"/>
-      <c r="AS67" s="112"/>
+      <c r="AR67" s="118"/>
+      <c r="AS67" s="119"/>
     </row>
     <row r="68" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="77"/>
-      <c r="B68" s="65">
+      <c r="A68" s="80"/>
+      <c r="B68" s="81">
         <v>32</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="66">
+      <c r="D68" s="77">
         <v>4</v>
       </c>
-      <c r="E68" s="67">
+      <c r="E68" s="68">
         <v>8</v>
       </c>
       <c r="F68" s="8"/>
@@ -5166,15 +5168,15 @@
       <c r="AO68" s="29"/>
       <c r="AP68" s="8"/>
       <c r="AQ68" s="9"/>
-      <c r="AR68" s="111"/>
-      <c r="AS68" s="112"/>
+      <c r="AR68" s="118"/>
+      <c r="AS68" s="119"/>
     </row>
     <row r="69" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="78"/>
-      <c r="B69" s="65"/>
-      <c r="C69" s="115"/>
-      <c r="D69" s="116"/>
-      <c r="E69" s="117"/>
+      <c r="A69" s="82"/>
+      <c r="B69" s="81"/>
+      <c r="C69" s="87"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="85"/>
       <c r="F69" s="16"/>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
@@ -5213,23 +5215,23 @@
       <c r="AO69" s="44"/>
       <c r="AP69" s="16"/>
       <c r="AQ69" s="17"/>
-      <c r="AR69" s="111"/>
-      <c r="AS69" s="112"/>
+      <c r="AR69" s="118"/>
+      <c r="AS69" s="119"/>
     </row>
     <row r="70" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="76" t="s">
+      <c r="A70" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="65">
+      <c r="B70" s="81">
         <v>33</v>
       </c>
-      <c r="C70" s="68" t="s">
+      <c r="C70" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="66">
+      <c r="D70" s="77">
         <v>1</v>
       </c>
-      <c r="E70" s="67">
+      <c r="E70" s="68">
         <v>1</v>
       </c>
       <c r="F70" s="8"/>
@@ -5270,15 +5272,15 @@
       <c r="AO70" s="10"/>
       <c r="AP70" s="8"/>
       <c r="AQ70" s="9"/>
-      <c r="AR70" s="111"/>
-      <c r="AS70" s="112"/>
+      <c r="AR70" s="118"/>
+      <c r="AS70" s="119"/>
     </row>
     <row r="71" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="77"/>
-      <c r="B71" s="65"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="66"/>
-      <c r="E71" s="67"/>
+      <c r="A71" s="80"/>
+      <c r="B71" s="81"/>
+      <c r="C71" s="83"/>
+      <c r="D71" s="77"/>
+      <c r="E71" s="68"/>
       <c r="F71" s="8"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
@@ -5317,21 +5319,21 @@
       <c r="AO71" s="57"/>
       <c r="AP71" s="8"/>
       <c r="AQ71" s="9"/>
-      <c r="AR71" s="111"/>
-      <c r="AS71" s="112"/>
+      <c r="AR71" s="118"/>
+      <c r="AS71" s="119"/>
     </row>
     <row r="72" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="77"/>
-      <c r="B72" s="65">
+      <c r="A72" s="80"/>
+      <c r="B72" s="81">
         <v>34</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="66">
+      <c r="D72" s="77">
         <v>1</v>
       </c>
-      <c r="E72" s="67"/>
+      <c r="E72" s="68"/>
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
@@ -5370,15 +5372,15 @@
       <c r="AO72" s="10"/>
       <c r="AP72" s="8"/>
       <c r="AQ72" s="9"/>
-      <c r="AR72" s="111"/>
-      <c r="AS72" s="112"/>
+      <c r="AR72" s="118"/>
+      <c r="AS72" s="119"/>
     </row>
     <row r="73" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="77"/>
-      <c r="B73" s="65"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="67"/>
+      <c r="A73" s="80"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="83"/>
+      <c r="D73" s="77"/>
+      <c r="E73" s="68"/>
       <c r="F73" s="8"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
@@ -5417,21 +5419,21 @@
       <c r="AO73" s="10"/>
       <c r="AP73" s="8"/>
       <c r="AQ73" s="9"/>
-      <c r="AR73" s="111"/>
-      <c r="AS73" s="112"/>
+      <c r="AR73" s="118"/>
+      <c r="AS73" s="119"/>
     </row>
     <row r="74" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="77"/>
-      <c r="B74" s="65">
+      <c r="A74" s="80"/>
+      <c r="B74" s="81">
         <v>35</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="66">
+      <c r="D74" s="77">
         <v>1</v>
       </c>
-      <c r="E74" s="67"/>
+      <c r="E74" s="68"/>
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
@@ -5470,15 +5472,15 @@
       <c r="AO74" s="10"/>
       <c r="AP74" s="8"/>
       <c r="AQ74" s="9"/>
-      <c r="AR74" s="111"/>
-      <c r="AS74" s="112"/>
+      <c r="AR74" s="118"/>
+      <c r="AS74" s="119"/>
     </row>
     <row r="75" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="77"/>
-      <c r="B75" s="65"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="67"/>
+      <c r="A75" s="80"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="77"/>
+      <c r="E75" s="68"/>
       <c r="F75" s="8"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
@@ -5517,21 +5519,21 @@
       <c r="AO75" s="10"/>
       <c r="AP75" s="8"/>
       <c r="AQ75" s="9"/>
-      <c r="AR75" s="111"/>
-      <c r="AS75" s="112"/>
+      <c r="AR75" s="118"/>
+      <c r="AS75" s="119"/>
     </row>
     <row r="76" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="77"/>
-      <c r="B76" s="65">
+      <c r="A76" s="80"/>
+      <c r="B76" s="81">
         <v>36</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="D76" s="66">
+      <c r="D76" s="77">
         <v>1</v>
       </c>
-      <c r="E76" s="67"/>
+      <c r="E76" s="68"/>
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
@@ -5570,15 +5572,15 @@
       <c r="AO76" s="10"/>
       <c r="AP76" s="32"/>
       <c r="AQ76" s="28"/>
-      <c r="AR76" s="111"/>
-      <c r="AS76" s="112"/>
+      <c r="AR76" s="118"/>
+      <c r="AS76" s="119"/>
     </row>
     <row r="77" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="77"/>
-      <c r="B77" s="65"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="66"/>
-      <c r="E77" s="67"/>
+      <c r="A77" s="80"/>
+      <c r="B77" s="81"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="77"/>
+      <c r="E77" s="68"/>
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
@@ -5617,21 +5619,21 @@
       <c r="AO77" s="10"/>
       <c r="AP77" s="8"/>
       <c r="AQ77" s="9"/>
-      <c r="AR77" s="111"/>
-      <c r="AS77" s="112"/>
+      <c r="AR77" s="118"/>
+      <c r="AS77" s="119"/>
     </row>
     <row r="78" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="77"/>
-      <c r="B78" s="65">
+      <c r="A78" s="80"/>
+      <c r="B78" s="81">
         <v>37</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="66">
+      <c r="D78" s="77">
         <v>1</v>
       </c>
-      <c r="E78" s="67"/>
+      <c r="E78" s="68"/>
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
@@ -5670,15 +5672,15 @@
       <c r="AO78" s="29"/>
       <c r="AP78" s="32"/>
       <c r="AQ78" s="28"/>
-      <c r="AR78" s="111"/>
-      <c r="AS78" s="112"/>
+      <c r="AR78" s="118"/>
+      <c r="AS78" s="119"/>
     </row>
     <row r="79" spans="1:45" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="78"/>
-      <c r="B79" s="65"/>
-      <c r="C79" s="115"/>
-      <c r="D79" s="116"/>
-      <c r="E79" s="117"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="87"/>
+      <c r="D79" s="84"/>
+      <c r="E79" s="85"/>
       <c r="F79" s="16"/>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
@@ -5717,8 +5719,8 @@
       <c r="AO79" s="44"/>
       <c r="AP79" s="16"/>
       <c r="AQ79" s="17"/>
-      <c r="AR79" s="113"/>
-      <c r="AS79" s="114"/>
+      <c r="AR79" s="120"/>
+      <c r="AS79" s="121"/>
     </row>
     <row r="80" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="50"/>
@@ -5731,88 +5733,255 @@
       </c>
       <c r="E80" s="21">
         <f>SUM(E4:E79)</f>
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AR80" s="22"/>
       <c r="AS80" s="22"/>
     </row>
     <row r="81" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A83" s="75" t="s">
+      <c r="A83" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="75"/>
+      <c r="B83" s="136"/>
       <c r="C83" s="49"/>
     </row>
     <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="74" t="s">
+      <c r="A85" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="74"/>
+      <c r="B85" s="67"/>
       <c r="C85" s="23"/>
     </row>
     <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="74" t="s">
+      <c r="A86" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="74"/>
+      <c r="B86" s="67"/>
       <c r="C86" s="24"/>
     </row>
     <row r="87" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="74" t="s">
+      <c r="A87" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="74"/>
+      <c r="B87" s="67"/>
       <c r="C87" s="11"/>
     </row>
     <row r="88" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="74" t="s">
+      <c r="A88" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B88" s="74"/>
+      <c r="B88" s="67"/>
       <c r="C88" s="56"/>
     </row>
     <row r="90" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="74" t="s">
+      <c r="A90" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B90" s="74"/>
+      <c r="B90" s="67"/>
       <c r="C90" s="47"/>
     </row>
     <row r="91" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="63" t="s">
+      <c r="A91" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="B91" s="64"/>
+      <c r="B91" s="133"/>
       <c r="C91" s="48"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="133" t="s">
+      <c r="A93" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="134"/>
+      <c r="B93" s="64"/>
       <c r="C93" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D93" s="135"/>
-      <c r="E93" s="135"/>
-      <c r="F93" s="135"/>
-      <c r="G93" s="135"/>
-      <c r="H93" s="135"/>
-      <c r="I93" s="135"/>
-      <c r="J93" s="135"/>
-      <c r="K93" s="135"/>
-      <c r="L93" s="135"/>
-      <c r="M93" s="135"/>
-      <c r="N93" s="135"/>
-      <c r="O93" s="135"/>
-      <c r="P93" s="135"/>
-      <c r="Q93" s="135"/>
-      <c r="R93" s="135"/>
-      <c r="S93" s="136"/>
+      <c r="D93" s="65"/>
+      <c r="E93" s="65"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="65"/>
+      <c r="H93" s="65"/>
+      <c r="I93" s="65"/>
+      <c r="J93" s="65"/>
+      <c r="K93" s="65"/>
+      <c r="L93" s="65"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
+      <c r="O93" s="65"/>
+      <c r="P93" s="65"/>
+      <c r="Q93" s="65"/>
+      <c r="R93" s="65"/>
+      <c r="S93" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="191">
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="A70:A79"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="AR4:AS79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="C44:C45"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="C50:C51"/>
@@ -5837,173 +6006,6 @@
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="AR4:AS79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="A70:A79"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="59" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>